<commit_message>
Adapt to last stack, fix missing adaptation, update template
</commit_message>
<xml_diff>
--- a/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
+++ b/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Introduction" sheetId="127" r:id="rId1"/>
     <sheet name="User Guidance" sheetId="126" r:id="rId2"/>
     <sheet name="Template" sheetId="125" r:id="rId3"/>
-    <sheet name="Lists" sheetId="41" r:id="rId4"/>
+    <sheet name="Lists" sheetId="41" state="hidden" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Template!$B$2:$G$206</definedName>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2313" uniqueCount="1052">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2314" uniqueCount="1053">
   <si>
     <t>Country</t>
   </si>
@@ -2691,9 +2691,6 @@
     <t>Solid manure from pigs, sows and piglets</t>
   </si>
   <si>
-    <t>Micronutrients</t>
-  </si>
-  <si>
     <r>
       <t>Harvest da</t>
     </r>
@@ -3478,6 +3475,12 @@
   </si>
   <si>
     <t>v2.0</t>
+  </si>
+  <si>
+    <t>Boric acid</t>
+  </si>
+  <si>
+    <t>Micro-/macronutrients</t>
   </si>
 </sst>
 </file>
@@ -6102,9 +6105,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6117,18 +6138,6 @@
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -6143,12 +6152,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="51" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="613">
@@ -8347,25 +8350,25 @@
     </row>
     <row r="5" spans="1:9" s="160" customFormat="1" ht="54.75" customHeight="1">
       <c r="A5" s="159"/>
-      <c r="B5" s="264"/>
-      <c r="C5" s="264"/>
-      <c r="D5" s="264"/>
-      <c r="E5" s="264"/>
-      <c r="F5" s="264"/>
-      <c r="G5" s="264"/>
+      <c r="B5" s="261"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
+      <c r="G5" s="261"/>
       <c r="H5" s="156"/>
       <c r="I5" s="156"/>
     </row>
     <row r="6" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A6" s="154"/>
-      <c r="B6" s="274" t="s">
-        <v>1051</v>
-      </c>
-      <c r="C6" s="265"/>
-      <c r="D6" s="265"/>
-      <c r="E6" s="265"/>
-      <c r="F6" s="265"/>
-      <c r="G6" s="265"/>
+      <c r="B6" s="262" t="s">
+        <v>1050</v>
+      </c>
+      <c r="C6" s="263"/>
+      <c r="D6" s="263"/>
+      <c r="E6" s="263"/>
+      <c r="F6" s="263"/>
+      <c r="G6" s="263"/>
       <c r="H6" s="156"/>
       <c r="I6" s="156"/>
     </row>
@@ -8382,14 +8385,14 @@
     </row>
     <row r="8" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A8" s="154"/>
-      <c r="B8" s="266" t="s">
+      <c r="B8" s="264" t="s">
         <v>708</v>
       </c>
-      <c r="C8" s="266"/>
-      <c r="D8" s="266"/>
-      <c r="E8" s="266"/>
-      <c r="F8" s="266"/>
-      <c r="G8" s="266"/>
+      <c r="C8" s="264"/>
+      <c r="D8" s="264"/>
+      <c r="E8" s="264"/>
+      <c r="F8" s="264"/>
+      <c r="G8" s="264"/>
       <c r="H8" s="161"/>
       <c r="I8" s="156"/>
     </row>
@@ -8406,14 +8409,14 @@
     </row>
     <row r="10" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A10" s="154"/>
-      <c r="B10" s="267" t="s">
+      <c r="B10" s="265" t="s">
         <v>772</v>
       </c>
-      <c r="C10" s="267"/>
-      <c r="D10" s="267"/>
-      <c r="E10" s="267"/>
-      <c r="F10" s="267"/>
-      <c r="G10" s="267"/>
+      <c r="C10" s="265"/>
+      <c r="D10" s="265"/>
+      <c r="E10" s="265"/>
+      <c r="F10" s="265"/>
+      <c r="G10" s="265"/>
       <c r="H10" s="156"/>
       <c r="I10" s="156"/>
     </row>
@@ -8421,10 +8424,10 @@
       <c r="A11" s="154"/>
       <c r="B11" s="173"/>
       <c r="C11" s="173"/>
-      <c r="D11" s="267"/>
-      <c r="E11" s="267"/>
-      <c r="F11" s="267"/>
-      <c r="G11" s="267"/>
+      <c r="D11" s="265"/>
+      <c r="E11" s="265"/>
+      <c r="F11" s="265"/>
+      <c r="G11" s="265"/>
       <c r="H11" s="156"/>
       <c r="I11" s="156"/>
     </row>
@@ -8434,12 +8437,12 @@
         <v>709</v>
       </c>
       <c r="C12" s="174"/>
-      <c r="D12" s="259" t="s">
+      <c r="D12" s="260" t="s">
         <v>710</v>
       </c>
-      <c r="E12" s="259"/>
-      <c r="F12" s="259"/>
-      <c r="G12" s="259"/>
+      <c r="E12" s="260"/>
+      <c r="F12" s="260"/>
+      <c r="G12" s="260"/>
       <c r="H12" s="156"/>
       <c r="I12" s="156"/>
     </row>
@@ -8449,12 +8452,12 @@
         <v>737</v>
       </c>
       <c r="C13" s="174"/>
-      <c r="D13" s="259" t="s">
+      <c r="D13" s="260" t="s">
         <v>739</v>
       </c>
-      <c r="E13" s="259"/>
-      <c r="F13" s="259"/>
-      <c r="G13" s="259"/>
+      <c r="E13" s="260"/>
+      <c r="F13" s="260"/>
+      <c r="G13" s="260"/>
       <c r="H13" s="156"/>
       <c r="I13" s="156"/>
     </row>
@@ -8464,12 +8467,12 @@
         <v>738</v>
       </c>
       <c r="C14" s="174"/>
-      <c r="D14" s="259" t="s">
+      <c r="D14" s="260" t="s">
         <v>740</v>
       </c>
-      <c r="E14" s="259"/>
-      <c r="F14" s="259"/>
-      <c r="G14" s="259"/>
+      <c r="E14" s="260"/>
+      <c r="F14" s="260"/>
+      <c r="G14" s="260"/>
       <c r="H14" s="156"/>
       <c r="I14" s="156"/>
     </row>
@@ -8477,10 +8480,10 @@
       <c r="A15" s="154"/>
       <c r="B15" s="175"/>
       <c r="C15" s="174"/>
-      <c r="D15" s="259"/>
-      <c r="E15" s="259"/>
-      <c r="F15" s="259"/>
-      <c r="G15" s="259"/>
+      <c r="D15" s="260"/>
+      <c r="E15" s="260"/>
+      <c r="F15" s="260"/>
+      <c r="G15" s="260"/>
       <c r="H15" s="156"/>
       <c r="I15" s="156"/>
     </row>
@@ -8497,23 +8500,23 @@
     </row>
     <row r="17" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A17" s="154"/>
-      <c r="B17" s="261" t="s">
+      <c r="B17" s="267" t="s">
         <v>711</v>
       </c>
-      <c r="C17" s="261"/>
-      <c r="D17" s="261"/>
-      <c r="E17" s="261"/>
-      <c r="F17" s="261"/>
-      <c r="G17" s="261"/>
+      <c r="C17" s="267"/>
+      <c r="D17" s="267"/>
+      <c r="E17" s="267"/>
+      <c r="F17" s="267"/>
+      <c r="G17" s="267"/>
       <c r="H17" s="161"/>
       <c r="I17" s="156"/>
     </row>
     <row r="18" spans="1:9" s="160" customFormat="1">
       <c r="A18" s="159"/>
-      <c r="B18" s="262" t="s">
+      <c r="B18" s="268" t="s">
         <v>712</v>
       </c>
-      <c r="C18" s="262"/>
+      <c r="C18" s="268"/>
       <c r="D18" s="180" t="s">
         <v>713</v>
       </c>
@@ -8531,10 +8534,10 @@
     </row>
     <row r="19" spans="1:9" s="160" customFormat="1">
       <c r="A19" s="159"/>
-      <c r="B19" s="263" t="s">
+      <c r="B19" s="269" t="s">
         <v>717</v>
       </c>
-      <c r="C19" s="263"/>
+      <c r="C19" s="269"/>
       <c r="D19" s="166" t="s">
         <v>718</v>
       </c>
@@ -8560,7 +8563,7 @@
         <v>781</v>
       </c>
       <c r="E20" s="167" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="F20" s="168" t="s">
         <v>782</v>
@@ -8573,10 +8576,10 @@
     </row>
     <row r="21" spans="1:9" s="160" customFormat="1">
       <c r="A21" s="159"/>
-      <c r="B21" s="260" t="s">
+      <c r="B21" s="266" t="s">
         <v>720</v>
       </c>
-      <c r="C21" s="260"/>
+      <c r="C21" s="266"/>
       <c r="D21" s="167" t="s">
         <v>721</v>
       </c>
@@ -8594,10 +8597,10 @@
     </row>
     <row r="22" spans="1:9" s="160" customFormat="1" ht="25.5">
       <c r="A22" s="159"/>
-      <c r="B22" s="260" t="s">
+      <c r="B22" s="266" t="s">
         <v>724</v>
       </c>
-      <c r="C22" s="260"/>
+      <c r="C22" s="266"/>
       <c r="D22" s="167" t="s">
         <v>725</v>
       </c>
@@ -8711,12 +8714,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="D11:G11"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="B21:C21"/>
@@ -8725,6 +8722,12 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <phoneticPr fontId="83" type="noConversion"/>
   <hyperlinks>
@@ -8746,8 +8749,8 @@
   </sheetPr>
   <dimension ref="A1:Z245"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <pane ySplit="5" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4:E4"/>
     </sheetView>
@@ -8779,12 +8782,12 @@
       </c>
     </row>
     <row r="2" spans="1:6" s="11" customFormat="1" ht="90" customHeight="1">
-      <c r="B2" s="268" t="s">
+      <c r="B2" s="270" t="s">
         <v>741</v>
       </c>
-      <c r="C2" s="268"/>
-      <c r="D2" s="268"/>
-      <c r="E2" s="268"/>
+      <c r="C2" s="270"/>
+      <c r="D2" s="270"/>
+      <c r="E2" s="270"/>
       <c r="F2" s="62"/>
     </row>
     <row r="3" spans="1:6" s="11" customFormat="1" ht="15.95" customHeight="1">
@@ -8799,10 +8802,10 @@
       <c r="C4" s="196" t="s">
         <v>742</v>
       </c>
-      <c r="D4" s="269" t="s">
+      <c r="D4" s="271" t="s">
         <v>774</v>
       </c>
-      <c r="E4" s="269"/>
+      <c r="E4" s="271"/>
       <c r="F4" s="63"/>
     </row>
     <row r="5" spans="1:6" s="11" customFormat="1" ht="30.95" customHeight="1">
@@ -8810,10 +8813,10 @@
       <c r="C5" s="196" t="s">
         <v>743</v>
       </c>
-      <c r="D5" s="270" t="s">
+      <c r="D5" s="272" t="s">
         <v>773</v>
       </c>
-      <c r="E5" s="270"/>
+      <c r="E5" s="272"/>
       <c r="F5" s="63"/>
     </row>
     <row r="6" spans="1:6" ht="8.1" customHeight="1">
@@ -9651,7 +9654,7 @@
     <row r="63" spans="1:6" outlineLevel="1" collapsed="1">
       <c r="A63" s="153"/>
       <c r="C63" s="32" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D63" s="142"/>
       <c r="E63" s="143"/>
@@ -9660,10 +9663,10 @@
     <row r="64" spans="1:6" outlineLevel="1">
       <c r="A64" s="153"/>
       <c r="C64" s="19" t="s">
+        <v>809</v>
+      </c>
+      <c r="D64" s="25" t="s">
         <v>810</v>
-      </c>
-      <c r="D64" s="25" t="s">
-        <v>811</v>
       </c>
       <c r="E64" s="13" t="s">
         <v>99</v>
@@ -9673,10 +9676,10 @@
     <row r="65" spans="1:6" outlineLevel="1">
       <c r="A65" s="153"/>
       <c r="C65" s="19" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D65" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E65" s="13" t="s">
         <v>99</v>
@@ -9686,10 +9689,10 @@
     <row r="66" spans="1:6" outlineLevel="1">
       <c r="A66" s="153"/>
       <c r="C66" s="19" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D66" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E66" s="13" t="s">
         <v>99</v>
@@ -9699,10 +9702,10 @@
     <row r="67" spans="1:6" outlineLevel="1">
       <c r="A67" s="153"/>
       <c r="C67" s="19" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D67" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E67" s="13" t="s">
         <v>99</v>
@@ -9712,10 +9715,10 @@
     <row r="68" spans="1:6" outlineLevel="1">
       <c r="A68" s="153"/>
       <c r="C68" s="19" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D68" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E68" s="13" t="s">
         <v>99</v>
@@ -9725,10 +9728,10 @@
     <row r="69" spans="1:6" outlineLevel="1">
       <c r="A69" s="153"/>
       <c r="C69" s="19" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D69" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E69" s="13" t="s">
         <v>99</v>
@@ -9776,7 +9779,7 @@
         <v>247</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D73" s="20" t="s">
         <v>22</v>
@@ -9816,7 +9819,7 @@
         <v>249</v>
       </c>
       <c r="C76" s="26" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="D76" s="27" t="s">
         <v>100</v>
@@ -9831,7 +9834,7 @@
         <v>250</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D77" s="27" t="s">
         <v>100</v>
@@ -9846,7 +9849,7 @@
         <v>251</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D78" s="27" t="s">
         <v>100</v>
@@ -9861,7 +9864,7 @@
         <v>252</v>
       </c>
       <c r="C79" s="19" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D79" s="27" t="s">
         <v>100</v>
@@ -10167,7 +10170,7 @@
         <v>31</v>
       </c>
       <c r="E100" s="214" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F100" s="64"/>
     </row>
@@ -10250,7 +10253,7 @@
         <v>290</v>
       </c>
       <c r="C106" s="46" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D106" s="23" t="s">
         <v>22</v>
@@ -10355,7 +10358,7 @@
         <v>287</v>
       </c>
       <c r="C113" s="46" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D113" s="23" t="s">
         <v>22</v>
@@ -10401,7 +10404,7 @@
         <v>300</v>
       </c>
       <c r="C116" s="46" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D116" s="23" t="s">
         <v>22</v>
@@ -10416,7 +10419,7 @@
         <v>299</v>
       </c>
       <c r="C117" s="46" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D117" s="23" t="s">
         <v>22</v>
@@ -10431,7 +10434,7 @@
         <v>302</v>
       </c>
       <c r="C118" s="46" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D118" s="23" t="s">
         <v>22</v>
@@ -10446,7 +10449,7 @@
         <v>298</v>
       </c>
       <c r="C119" s="46" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D119" s="23" t="s">
         <v>22</v>
@@ -10461,7 +10464,7 @@
         <v>301</v>
       </c>
       <c r="C120" s="46" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D120" s="23" t="s">
         <v>22</v>
@@ -10476,7 +10479,7 @@
         <v>297</v>
       </c>
       <c r="C121" s="46" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D121" s="23" t="s">
         <v>22</v>
@@ -10491,7 +10494,7 @@
         <v>296</v>
       </c>
       <c r="C122" s="46" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D122" s="23" t="s">
         <v>22</v>
@@ -10995,7 +10998,7 @@
         <v>52</v>
       </c>
       <c r="E156" s="222" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="F156" s="64"/>
     </row>
@@ -11308,7 +11311,7 @@
       </c>
       <c r="B181" s="7"/>
       <c r="C181" s="5" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="D181" s="7" t="s">
         <v>27</v>
@@ -11342,7 +11345,7 @@
       </c>
       <c r="B183" s="12"/>
       <c r="C183" s="29" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="D183" s="12" t="s">
         <v>27</v>
@@ -11415,7 +11418,7 @@
       </c>
       <c r="B187" s="12"/>
       <c r="C187" s="29" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="D187" s="12" t="s">
         <v>27</v>
@@ -11488,7 +11491,7 @@
       </c>
       <c r="B191" s="12"/>
       <c r="C191" s="134" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="D191" s="139" t="s">
         <v>27</v>
@@ -11561,7 +11564,7 @@
       </c>
       <c r="B195" s="12"/>
       <c r="C195" s="29" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="D195" s="12" t="s">
         <v>27</v>
@@ -11635,7 +11638,7 @@
       </c>
       <c r="B199" s="12"/>
       <c r="C199" s="134" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="D199" s="12" t="s">
         <v>27</v>
@@ -11709,7 +11712,7 @@
       </c>
       <c r="B203" s="12"/>
       <c r="C203" s="134" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="D203" s="139" t="s">
         <v>27</v>
@@ -11766,7 +11769,7 @@
       </c>
       <c r="B206" s="120"/>
       <c r="C206" s="122" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D206" s="123" t="s">
         <v>8</v>
@@ -11826,7 +11829,7 @@
       </c>
       <c r="B209" s="12"/>
       <c r="C209" s="26" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D209" s="7" t="s">
         <v>142</v>
@@ -11847,7 +11850,7 @@
       </c>
       <c r="B210" s="12"/>
       <c r="C210" s="26" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D210" s="7" t="s">
         <v>142</v>
@@ -12282,7 +12285,7 @@
     <row r="223" spans="1:26" s="198" customFormat="1" ht="20.100000000000001" customHeight="1">
       <c r="B223" s="199"/>
       <c r="C223" s="204" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D223" s="228" t="s">
         <v>8</v>
@@ -12345,7 +12348,7 @@
       </c>
       <c r="B226" s="12"/>
       <c r="C226" s="26" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="D226" s="7" t="s">
         <v>32</v>
@@ -12398,7 +12401,7 @@
         <v>27</v>
       </c>
       <c r="E229" s="223" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F229" s="64"/>
     </row>
@@ -12546,7 +12549,7 @@
     <row r="239" spans="1:26" s="86" customFormat="1" ht="35.1" customHeight="1">
       <c r="B239" s="88"/>
       <c r="C239" s="124" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D239" s="125" t="s">
         <v>8</v>
@@ -12644,7 +12647,7 @@
       </c>
       <c r="B243" s="12"/>
       <c r="C243" s="26" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D243" s="86" t="s">
         <v>32</v>
@@ -12665,7 +12668,7 @@
       </c>
       <c r="B244" s="12"/>
       <c r="C244" s="26" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D244" s="86" t="s">
         <v>32</v>
@@ -12686,10 +12689,10 @@
       </c>
       <c r="B245" s="12"/>
       <c r="C245" s="26" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D245" s="86" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E245" s="223" t="s">
         <v>99</v>
@@ -12779,7 +12782,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$O$2:$O$107</xm:f>
+            <xm:f>Lists!$O$2:$O$108</xm:f>
           </x14:formula1>
           <xm:sqref>C173:C175</xm:sqref>
         </x14:dataValidation>
@@ -12800,7 +12803,7 @@
     <sheetView workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="E12" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -12819,7 +12822,7 @@
   <sheetData>
     <row r="1" spans="1:8" hidden="1">
       <c r="A1" s="98" t="s">
-        <v>1050</v>
+        <v>1049</v>
       </c>
       <c r="C1" s="100" t="s">
         <v>236</v>
@@ -12838,14 +12841,14 @@
       </c>
     </row>
     <row r="2" spans="1:8" s="11" customFormat="1" ht="78" customHeight="1">
-      <c r="B2" s="268" t="s">
+      <c r="B2" s="270" t="s">
         <v>741</v>
       </c>
-      <c r="C2" s="268"/>
-      <c r="D2" s="268"/>
-      <c r="E2" s="268"/>
-      <c r="F2" s="268"/>
-      <c r="G2" s="268"/>
+      <c r="C2" s="270"/>
+      <c r="D2" s="270"/>
+      <c r="E2" s="270"/>
+      <c r="F2" s="270"/>
+      <c r="G2" s="270"/>
       <c r="H2" s="62"/>
     </row>
     <row r="3" spans="1:8" s="11" customFormat="1" ht="15.95" customHeight="1">
@@ -12859,34 +12862,34 @@
     </row>
     <row r="4" spans="1:8" ht="21">
       <c r="A4" s="153" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="B4" s="188"/>
       <c r="C4" s="192" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="D4" s="190" t="s">
         <v>660</v>
       </c>
-      <c r="E4" s="271"/>
-      <c r="F4" s="271"/>
-      <c r="G4" s="271"/>
+      <c r="E4" s="273"/>
+      <c r="F4" s="273"/>
+      <c r="G4" s="273"/>
       <c r="H4" s="64"/>
     </row>
     <row r="5" spans="1:8" ht="21">
       <c r="A5" s="153" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="B5" s="189"/>
       <c r="C5" s="193" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="D5" s="191" t="s">
         <v>661</v>
       </c>
-      <c r="E5" s="272"/>
-      <c r="F5" s="272"/>
-      <c r="G5" s="272"/>
+      <c r="E5" s="274"/>
+      <c r="F5" s="274"/>
+      <c r="G5" s="274"/>
       <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:8" ht="8.1" customHeight="1">
@@ -13016,7 +13019,7 @@
     <row r="14" spans="1:8" outlineLevel="1">
       <c r="A14" s="153"/>
       <c r="C14" s="32" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="D14" s="142"/>
       <c r="E14" s="143"/>
@@ -13026,13 +13029,13 @@
     </row>
     <row r="15" spans="1:8" outlineLevel="1">
       <c r="A15" s="153" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C15" s="19" t="s">
+        <v>809</v>
+      </c>
+      <c r="D15" s="25" t="s">
         <v>810</v>
-      </c>
-      <c r="D15" s="25" t="s">
-        <v>811</v>
       </c>
       <c r="E15" s="33" t="s">
         <v>99</v>
@@ -13043,13 +13046,13 @@
     </row>
     <row r="16" spans="1:8" outlineLevel="1">
       <c r="A16" s="153" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="D16" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E16" s="33" t="s">
         <v>99</v>
@@ -13060,13 +13063,13 @@
     </row>
     <row r="17" spans="1:8" outlineLevel="1">
       <c r="A17" s="153" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="D17" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E17" s="33" t="s">
         <v>99</v>
@@ -13077,13 +13080,13 @@
     </row>
     <row r="18" spans="1:8" outlineLevel="1">
       <c r="A18" s="153" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="D18" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E18" s="33" t="s">
         <v>99</v>
@@ -13094,13 +13097,13 @@
     </row>
     <row r="19" spans="1:8" outlineLevel="1">
       <c r="A19" s="153" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="D19" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E19" s="33" t="s">
         <v>99</v>
@@ -13111,13 +13114,13 @@
     </row>
     <row r="20" spans="1:8" outlineLevel="1">
       <c r="A20" s="153" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="D20" s="25" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="E20" s="33" t="s">
         <v>99</v>
@@ -13147,7 +13150,7 @@
     </row>
     <row r="22" spans="1:8" outlineLevel="1">
       <c r="C22" s="32" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="D22" s="142"/>
       <c r="E22" s="143"/>
@@ -13157,17 +13160,17 @@
     </row>
     <row r="23" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A23" s="254" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B23" s="12"/>
       <c r="C23" s="19" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="D23" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E23" s="33" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="F23" s="3"/>
       <c r="G23" s="3"/>
@@ -13175,17 +13178,17 @@
     </row>
     <row r="24" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A24" s="254" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B24" s="12"/>
       <c r="C24" s="19" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="D24" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="F24" s="3"/>
       <c r="G24" s="3"/>
@@ -13213,7 +13216,7 @@
         <v>247</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="D26" s="20" t="s">
         <v>22</v>
@@ -13227,11 +13230,11 @@
     </row>
     <row r="27" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A27" s="252" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B27" s="12"/>
       <c r="C27" s="19" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="D27" s="20" t="s">
         <v>28</v>
@@ -13245,14 +13248,14 @@
     </row>
     <row r="28" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A28" s="252" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="B28" s="12"/>
       <c r="C28" s="19" t="s">
+        <v>979</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>980</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>981</v>
       </c>
       <c r="E28" s="22" t="s">
         <v>99</v>
@@ -13264,7 +13267,7 @@
     <row r="29" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="B29" s="12"/>
       <c r="C29" s="32" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="D29" s="20"/>
       <c r="E29" s="22"/>
@@ -13274,17 +13277,17 @@
     </row>
     <row r="30" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A30" s="252" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="B30" s="12"/>
       <c r="C30" s="19" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="D30" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E30" s="22" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="F30" s="21"/>
       <c r="G30" s="3"/>
@@ -13292,17 +13295,17 @@
     </row>
     <row r="31" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A31" s="252" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="B31" s="12"/>
       <c r="C31" s="19" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="D31" s="25" t="s">
         <v>21</v>
       </c>
       <c r="E31" s="22" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="F31" s="21"/>
       <c r="G31" s="3"/>
@@ -13340,7 +13343,7 @@
         <v>249</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="D34" s="27" t="s">
         <v>100</v>
@@ -13357,7 +13360,7 @@
         <v>250</v>
       </c>
       <c r="C35" s="19" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="D35" s="27" t="s">
         <v>100</v>
@@ -13374,7 +13377,7 @@
         <v>251</v>
       </c>
       <c r="C36" s="19" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="D36" s="27" t="s">
         <v>100</v>
@@ -13391,7 +13394,7 @@
         <v>252</v>
       </c>
       <c r="C37" s="19" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="D37" s="27" t="s">
         <v>100</v>
@@ -13456,11 +13459,11 @@
     </row>
     <row r="41" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A41" s="252" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="26" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>28</v>
@@ -13756,7 +13759,7 @@
     </row>
     <row r="59" spans="1:8" outlineLevel="1">
       <c r="C59" s="41" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="108"/>
@@ -13770,7 +13773,7 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="46" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>31</v>
@@ -13785,7 +13788,7 @@
     <row r="61" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="B61" s="12"/>
       <c r="C61" s="41" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="108"/>
@@ -13795,11 +13798,11 @@
     </row>
     <row r="62" spans="1:8" s="252" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A62" s="252" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="46" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>31</v>
@@ -13813,11 +13816,11 @@
     </row>
     <row r="63" spans="1:8" s="252" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A63" s="252" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="46" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>31</v>
@@ -13831,11 +13834,11 @@
     </row>
     <row r="64" spans="1:8" s="252" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A64" s="252" t="s">
-        <v>1005</v>
+        <v>1004</v>
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="46" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>31</v>
@@ -13941,7 +13944,7 @@
         <v>290</v>
       </c>
       <c r="C70" s="46" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="D70" s="39" t="s">
         <v>22</v>
@@ -14060,7 +14063,7 @@
         <v>287</v>
       </c>
       <c r="C77" s="46" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="D77" s="39" t="s">
         <v>22</v>
@@ -14113,7 +14116,7 @@
         <v>300</v>
       </c>
       <c r="C80" s="238" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="D80" s="39" t="s">
         <v>22</v>
@@ -14130,7 +14133,7 @@
         <v>299</v>
       </c>
       <c r="C81" s="238" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="D81" s="39" t="s">
         <v>22</v>
@@ -14147,7 +14150,7 @@
         <v>302</v>
       </c>
       <c r="C82" s="46" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="D82" s="39" t="s">
         <v>22</v>
@@ -14164,7 +14167,7 @@
         <v>298</v>
       </c>
       <c r="C83" s="238" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="D83" s="39" t="s">
         <v>22</v>
@@ -14181,7 +14184,7 @@
         <v>301</v>
       </c>
       <c r="C84" s="46" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="D84" s="39" t="s">
         <v>22</v>
@@ -14198,7 +14201,7 @@
         <v>297</v>
       </c>
       <c r="C85" s="46" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="D85" s="39" t="s">
         <v>22</v>
@@ -14215,7 +14218,7 @@
         <v>296</v>
       </c>
       <c r="C86" s="46" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="D86" s="39" t="s">
         <v>22</v>
@@ -14334,7 +14337,7 @@
     <row r="93" spans="1:8" ht="21">
       <c r="B93" s="70"/>
       <c r="C93" s="71" t="s">
-        <v>804</v>
+        <v>1052</v>
       </c>
       <c r="D93" s="72" t="s">
         <v>8</v>
@@ -14454,14 +14457,14 @@
     </row>
     <row r="100" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A100" s="252" t="s">
-        <v>1011</v>
+        <v>1010</v>
       </c>
       <c r="B100" s="12"/>
       <c r="C100" s="30" t="s">
+        <v>1005</v>
+      </c>
+      <c r="D100" s="7" t="s">
         <v>1006</v>
-      </c>
-      <c r="D100" s="7" t="s">
-        <v>1007</v>
       </c>
       <c r="E100" s="109" t="s">
         <v>99</v>
@@ -14472,11 +14475,11 @@
     </row>
     <row r="101" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A101" s="252" t="s">
-        <v>1012</v>
+        <v>1011</v>
       </c>
       <c r="B101" s="12"/>
       <c r="C101" s="46" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="D101" s="39" t="s">
         <v>22</v>
@@ -14490,11 +14493,11 @@
     </row>
     <row r="102" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A102" s="252" t="s">
-        <v>1013</v>
+        <v>1012</v>
       </c>
       <c r="B102" s="12"/>
       <c r="C102" s="46" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="D102" s="39" t="s">
         <v>22</v>
@@ -14508,11 +14511,11 @@
     </row>
     <row r="103" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A103" s="252" t="s">
-        <v>1014</v>
+        <v>1013</v>
       </c>
       <c r="B103" s="12"/>
       <c r="C103" s="46" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="D103" s="39" t="s">
         <v>22</v>
@@ -14527,7 +14530,7 @@
     <row r="104" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="B104" s="12"/>
       <c r="C104" s="30" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="109"/>
@@ -14537,11 +14540,11 @@
     </row>
     <row r="105" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A105" s="252" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="B105" s="12"/>
       <c r="C105" s="46" t="s">
-        <v>1016</v>
+        <v>1015</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>27</v>
@@ -14555,11 +14558,11 @@
     </row>
     <row r="106" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A106" s="252" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="B106" s="12"/>
       <c r="C106" s="46" t="s">
-        <v>1017</v>
+        <v>1016</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>27</v>
@@ -14573,11 +14576,11 @@
     </row>
     <row r="107" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A107" s="252" t="s">
-        <v>1024</v>
+        <v>1023</v>
       </c>
       <c r="B107" s="12"/>
       <c r="C107" s="46" t="s">
-        <v>1018</v>
+        <v>1017</v>
       </c>
       <c r="D107" s="7" t="s">
         <v>27</v>
@@ -14591,11 +14594,11 @@
     </row>
     <row r="108" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A108" s="252" t="s">
-        <v>1025</v>
+        <v>1024</v>
       </c>
       <c r="B108" s="12"/>
       <c r="C108" s="46" t="s">
-        <v>1019</v>
+        <v>1018</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>27</v>
@@ -14609,11 +14612,11 @@
     </row>
     <row r="109" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A109" s="252" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="B109" s="12"/>
       <c r="C109" s="46" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="D109" s="7" t="s">
         <v>27</v>
@@ -14627,11 +14630,11 @@
     </row>
     <row r="110" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A110" s="252" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="B110" s="12"/>
       <c r="C110" s="46" t="s">
-        <v>1021</v>
+        <v>1020</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>27</v>
@@ -14698,7 +14701,7 @@
     </row>
     <row r="114" spans="1:8" outlineLevel="1">
       <c r="A114" s="250" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C114" s="236" t="s">
         <v>795</v>
@@ -14732,7 +14735,7 @@
     </row>
     <row r="116" spans="1:8" outlineLevel="1">
       <c r="A116" s="250" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C116" s="236" t="s">
         <v>797</v>
@@ -15387,7 +15390,7 @@
       </c>
       <c r="B156" s="7"/>
       <c r="C156" s="5" t="s">
-        <v>1028</v>
+        <v>1027</v>
       </c>
       <c r="D156" s="7" t="s">
         <v>27</v>
@@ -15429,7 +15432,7 @@
       </c>
       <c r="B158" s="12"/>
       <c r="C158" s="29" t="s">
-        <v>1029</v>
+        <v>1028</v>
       </c>
       <c r="D158" s="12" t="s">
         <v>27</v>
@@ -15514,7 +15517,7 @@
       </c>
       <c r="B162" s="12"/>
       <c r="C162" s="29" t="s">
-        <v>1030</v>
+        <v>1029</v>
       </c>
       <c r="D162" s="12" t="s">
         <v>27</v>
@@ -15599,7 +15602,7 @@
       </c>
       <c r="B166" s="12"/>
       <c r="C166" s="134" t="s">
-        <v>1031</v>
+        <v>1030</v>
       </c>
       <c r="D166" s="139" t="s">
         <v>27</v>
@@ -15684,7 +15687,7 @@
       </c>
       <c r="B170" s="12"/>
       <c r="C170" s="29" t="s">
-        <v>1032</v>
+        <v>1031</v>
       </c>
       <c r="D170" s="12" t="s">
         <v>27</v>
@@ -15770,7 +15773,7 @@
       </c>
       <c r="B174" s="12"/>
       <c r="C174" s="134" t="s">
-        <v>1033</v>
+        <v>1032</v>
       </c>
       <c r="D174" s="12" t="s">
         <v>27</v>
@@ -15856,7 +15859,7 @@
       </c>
       <c r="B178" s="12"/>
       <c r="C178" s="134" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="D178" s="139" t="s">
         <v>27</v>
@@ -15919,7 +15922,7 @@
       </c>
       <c r="B181" s="117"/>
       <c r="C181" s="117" t="s">
-        <v>1035</v>
+        <v>1034</v>
       </c>
       <c r="D181" s="118" t="s">
         <v>8</v>
@@ -15937,11 +15940,11 @@
     </row>
     <row r="182" spans="1:28" s="253" customFormat="1" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="A182" s="253" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="B182" s="12"/>
       <c r="C182" s="134" t="s">
-        <v>1037</v>
+        <v>1036</v>
       </c>
       <c r="D182" s="139" t="s">
         <v>27</v>
@@ -15962,7 +15965,7 @@
       <c r="A183" s="11"/>
       <c r="B183" s="120"/>
       <c r="C183" s="122" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="D183" s="123" t="s">
         <v>8</v>
@@ -16036,7 +16039,7 @@
       </c>
       <c r="B186" s="12"/>
       <c r="C186" s="26" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="D186" s="7" t="s">
         <v>142</v>
@@ -16059,7 +16062,7 @@
       </c>
       <c r="B187" s="12"/>
       <c r="C187" s="26" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="D187" s="7" t="s">
         <v>142</v>
@@ -16524,7 +16527,7 @@
     <row r="200" spans="1:28" ht="20.100000000000001" customHeight="1">
       <c r="B200" s="197"/>
       <c r="C200" s="204" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="D200" s="228" t="s">
         <v>8</v>
@@ -16547,7 +16550,7 @@
     </row>
     <row r="201" spans="1:28" s="9" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A201" s="252" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="B201" s="12"/>
       <c r="C201" s="26" t="s">
@@ -16570,7 +16573,7 @@
     </row>
     <row r="202" spans="1:28" s="9" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A202" s="252" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="B202" s="12"/>
       <c r="C202" s="26" t="s">
@@ -16593,7 +16596,7 @@
     </row>
     <row r="203" spans="1:28" s="9" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A203" s="252" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="B203" s="12"/>
       <c r="C203" s="26" t="s">
@@ -16763,11 +16766,11 @@
     </row>
     <row r="212" spans="1:28" outlineLevel="1">
       <c r="A212" s="4" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="B212" s="7"/>
       <c r="C212" s="26" t="s">
-        <v>1038</v>
+        <v>1037</v>
       </c>
       <c r="D212" s="7" t="s">
         <v>90</v>
@@ -16781,11 +16784,11 @@
     </row>
     <row r="213" spans="1:28" outlineLevel="1">
       <c r="A213" s="4" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="B213" s="7"/>
       <c r="C213" s="26" t="s">
-        <v>1039</v>
+        <v>1038</v>
       </c>
       <c r="D213" s="7" t="s">
         <v>90</v>
@@ -16800,7 +16803,7 @@
     <row r="214" spans="1:28" s="86" customFormat="1" ht="35.1" customHeight="1">
       <c r="B214" s="88"/>
       <c r="C214" s="124" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="D214" s="125" t="s">
         <v>8</v>
@@ -16837,7 +16840,7 @@
     </row>
     <row r="215" spans="1:28" s="87" customFormat="1" outlineLevel="1">
       <c r="A215" s="87" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="B215" s="12"/>
       <c r="C215" s="26" t="s">
@@ -16860,7 +16863,7 @@
     </row>
     <row r="216" spans="1:28" s="87" customFormat="1" outlineLevel="1">
       <c r="A216" s="87" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="B216" s="12"/>
       <c r="C216" s="150" t="s">
@@ -16883,7 +16886,7 @@
     </row>
     <row r="217" spans="1:28" s="87" customFormat="1" outlineLevel="1">
       <c r="A217" s="87" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="B217" s="12"/>
       <c r="C217" s="150" t="s">
@@ -16906,11 +16909,11 @@
     </row>
     <row r="218" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A218" s="11" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="B218" s="12"/>
       <c r="C218" s="26" t="s">
-        <v>1042</v>
+        <v>1041</v>
       </c>
       <c r="D218" s="86" t="s">
         <v>27</v>
@@ -16929,7 +16932,7 @@
     </row>
     <row r="219" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A219" s="11" t="s">
-        <v>1046</v>
+        <v>1045</v>
       </c>
       <c r="B219" s="12"/>
       <c r="C219" s="150" t="s">
@@ -16952,11 +16955,11 @@
     </row>
     <row r="220" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A220" s="11" t="s">
-        <v>1047</v>
+        <v>1046</v>
       </c>
       <c r="B220" s="12"/>
       <c r="C220" s="150" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="D220" s="86" t="s">
         <v>22</v>
@@ -16975,11 +16978,11 @@
     </row>
     <row r="221" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A221" s="11" t="s">
-        <v>1048</v>
+        <v>1047</v>
       </c>
       <c r="B221" s="12"/>
       <c r="C221" s="150" t="s">
-        <v>1044</v>
+        <v>1043</v>
       </c>
       <c r="D221" s="86" t="s">
         <v>22</v>
@@ -16998,11 +17001,11 @@
     </row>
     <row r="222" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A222" s="11" t="s">
-        <v>1049</v>
+        <v>1048</v>
       </c>
       <c r="B222" s="12"/>
       <c r="C222" s="150" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D222" s="86" t="s">
         <v>22</v>
@@ -17021,11 +17024,11 @@
     </row>
     <row r="223" spans="1:28" s="87" customFormat="1" outlineLevel="1">
       <c r="A223" s="253" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="B223" s="12"/>
       <c r="C223" s="26" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="D223" s="86" t="s">
         <v>32</v>
@@ -17044,11 +17047,11 @@
     </row>
     <row r="224" spans="1:28" s="87" customFormat="1" outlineLevel="1">
       <c r="A224" s="253" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="B224" s="12"/>
       <c r="C224" s="26" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="D224" s="86" t="s">
         <v>32</v>
@@ -17067,14 +17070,14 @@
     </row>
     <row r="225" spans="1:13" s="87" customFormat="1" outlineLevel="1">
       <c r="A225" s="253" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="B225" s="12"/>
       <c r="C225" s="26" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="D225" s="86" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="E225" s="111" t="s">
         <v>99</v>
@@ -17184,12 +17187,6 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$O$2:$O$107</xm:f>
-          </x14:formula1>
-          <xm:sqref>C148:C150</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>Lists!$M$2:$M$141</xm:f>
           </x14:formula1>
           <xm:sqref>C134:C136</xm:sqref>
@@ -17218,6 +17215,12 @@
           </x14:formula1>
           <xm:sqref>E31</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$O$2:$O$108</xm:f>
+          </x14:formula1>
+          <xm:sqref>C148:C150</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -17232,9 +17235,9 @@
   <dimension ref="A1:V141"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B35" sqref="B35"/>
-      <selection pane="bottomLeft" activeCell="U2" sqref="U2"/>
+      <selection pane="bottomLeft" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17289,26 +17292,26 @@
         <v>786</v>
       </c>
       <c r="P1" s="235" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="Q1" s="235" t="s">
+        <v>942</v>
+      </c>
+      <c r="R1" s="235" t="s">
         <v>943</v>
       </c>
-      <c r="R1" s="235" t="s">
+      <c r="S1" s="235" t="s">
         <v>944</v>
-      </c>
-      <c r="S1" s="235" t="s">
-        <v>945</v>
       </c>
       <c r="T1" s="235" t="str">
         <f>Template!E23</f>
         <v>&lt;select climate zone 1&gt;</v>
       </c>
       <c r="U1" s="235" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="V1" s="235" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
     </row>
     <row r="2" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -17358,25 +17361,25 @@
         <v>369</v>
       </c>
       <c r="P2" s="258" t="s">
+        <v>974</v>
+      </c>
+      <c r="Q2" s="258" t="s">
         <v>975</v>
       </c>
-      <c r="Q2" s="258" t="s">
-        <v>976</v>
-      </c>
       <c r="R2" s="258" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="S2" s="258" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="T2" s="258" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="U2" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="V2" s="258" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
     </row>
     <row r="3" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -17390,7 +17393,7 @@
         <v>167</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>168</v>
@@ -17420,32 +17423,32 @@
         <v>371</v>
       </c>
       <c r="N3" s="256" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="O3" s="256" t="s">
         <v>574</v>
       </c>
       <c r="P3" s="258" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="Q3" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="R3" s="1" t="s">
         <v>949</v>
       </c>
-      <c r="R3" s="1" t="s">
+      <c r="S3" s="1" t="s">
         <v>950</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>951</v>
       </c>
       <c r="T3" s="1" t="str">
         <f>IF(T$1=P$3,Q3,IF(T$1=P$4,R3,IF(T$1=P$5,S3,"")))</f>
         <v/>
       </c>
       <c r="U3" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="V3" s="258" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
     </row>
     <row r="4" spans="1:22" s="1" customFormat="1" ht="27" thickBot="1">
@@ -17494,24 +17497,24 @@
       <c r="O4" s="256" t="s">
         <v>575</v>
       </c>
-      <c r="P4" s="273" t="s">
-        <v>947</v>
+      <c r="P4" s="259" t="s">
+        <v>946</v>
       </c>
       <c r="Q4" s="1" t="s">
+        <v>951</v>
+      </c>
+      <c r="R4" s="1" t="s">
         <v>952</v>
       </c>
-      <c r="R4" s="1" t="s">
+      <c r="S4" s="1" t="s">
         <v>953</v>
-      </c>
-      <c r="S4" s="1" t="s">
-        <v>954</v>
       </c>
       <c r="T4" s="258" t="str">
         <f t="shared" ref="T4:T17" si="0">IF(T$1=P$3,Q4,IF(T$1=P$4,R4,IF(T$1=P$5,S4,"")))</f>
         <v/>
       </c>
       <c r="U4" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="1" customFormat="1" ht="27" thickBot="1">
@@ -17522,7 +17525,7 @@
         <v>121</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>180</v>
@@ -17555,22 +17558,22 @@
         <v>373</v>
       </c>
       <c r="N5" s="256" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="O5" s="256" t="s">
         <v>576</v>
       </c>
-      <c r="P5" s="273" t="s">
-        <v>948</v>
+      <c r="P5" s="259" t="s">
+        <v>947</v>
       </c>
       <c r="Q5" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>955</v>
       </c>
-      <c r="R5" s="1" t="s">
+      <c r="S5" s="1" t="s">
         <v>956</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>957</v>
       </c>
       <c r="T5" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17591,7 +17594,7 @@
         <v>187</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>188</v>
@@ -17612,19 +17615,19 @@
         <v>374</v>
       </c>
       <c r="N6" s="256" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="O6" s="256" t="s">
         <v>577</v>
       </c>
       <c r="Q6" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="R6" s="1" t="s">
         <v>958</v>
       </c>
-      <c r="R6" s="1" t="s">
+      <c r="S6" s="1" t="s">
         <v>959</v>
-      </c>
-      <c r="S6" s="1" t="s">
-        <v>960</v>
       </c>
       <c r="T6" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17642,13 +17645,13 @@
         <v>191</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>192</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I7" s="258" t="s">
         <v>193</v>
@@ -17669,10 +17672,10 @@
         <v>578</v>
       </c>
       <c r="R7" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="S7" s="1" t="s">
         <v>961</v>
-      </c>
-      <c r="S7" s="1" t="s">
-        <v>962</v>
       </c>
       <c r="T7" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17690,7 +17693,7 @@
         <v>196</v>
       </c>
       <c r="I8" s="257" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="J8" s="1" t="s">
         <v>60</v>
@@ -17705,13 +17708,13 @@
         <v>492</v>
       </c>
       <c r="O8" s="256" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="R8" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="S8" s="1" t="s">
         <v>963</v>
-      </c>
-      <c r="S8" s="1" t="s">
-        <v>964</v>
       </c>
       <c r="T8" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17726,7 +17729,7 @@
         <v>199</v>
       </c>
       <c r="I9" s="257" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>61</v>
@@ -17735,7 +17738,7 @@
         <v>361</v>
       </c>
       <c r="M9" s="256" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="N9" s="256" t="s">
         <v>493</v>
@@ -17744,10 +17747,10 @@
         <v>579</v>
       </c>
       <c r="R9" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="S9" s="1" t="s">
         <v>965</v>
-      </c>
-      <c r="S9" s="1" t="s">
-        <v>966</v>
       </c>
       <c r="T9" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17780,7 +17783,7 @@
         <v>580</v>
       </c>
       <c r="R10" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="T10" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17795,7 +17798,7 @@
         <v>205</v>
       </c>
       <c r="I11" s="257" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>63</v>
@@ -17813,7 +17816,7 @@
         <v>581</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="T11" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17822,19 +17825,19 @@
     </row>
     <row r="12" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="D12" s="1" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>207</v>
       </c>
       <c r="I12" s="257" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>59</v>
       </c>
       <c r="M12" s="256" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="N12" s="256" t="s">
         <v>496</v>
@@ -17843,7 +17846,7 @@
         <v>582</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="T12" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17855,7 +17858,7 @@
         <v>208</v>
       </c>
       <c r="I13" s="257" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>65</v>
@@ -17870,7 +17873,7 @@
         <v>583</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="T13" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17879,7 +17882,7 @@
     </row>
     <row r="14" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="G14" s="9" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="I14" s="258" t="s">
         <v>200</v>
@@ -17897,7 +17900,7 @@
         <v>584</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="T14" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17915,13 +17918,13 @@
         <v>381</v>
       </c>
       <c r="N15" s="256" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="O15" s="256" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="T15" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17936,7 +17939,7 @@
         <v>64</v>
       </c>
       <c r="M16" s="256" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="N16" s="256" t="s">
         <v>499</v>
@@ -17945,7 +17948,7 @@
         <v>650</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="T16" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17954,7 +17957,7 @@
     </row>
     <row r="17" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I17" s="257" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>69</v>
@@ -17966,10 +17969,10 @@
         <v>500</v>
       </c>
       <c r="O17" s="256" t="s">
-        <v>585</v>
+        <v>1051</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="T17" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17978,7 +17981,7 @@
     </row>
     <row r="18" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I18" s="257" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>70</v>
@@ -17990,29 +17993,29 @@
         <v>501</v>
       </c>
       <c r="O18" s="256" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="19" spans="9:20" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I19" s="257" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>73</v>
       </c>
       <c r="M19" s="256" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="N19" s="256" t="s">
         <v>502</v>
       </c>
       <c r="O19" s="256" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="20" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I20" s="257" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>71</v>
@@ -18024,12 +18027,12 @@
         <v>503</v>
       </c>
       <c r="O20" s="256" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="21" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I21" s="257" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>72</v>
@@ -18041,12 +18044,12 @@
         <v>537</v>
       </c>
       <c r="O21" s="256" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="22" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I22" s="257" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>74</v>
@@ -18058,7 +18061,7 @@
         <v>504</v>
       </c>
       <c r="O22" s="256" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="23" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18075,12 +18078,12 @@
         <v>505</v>
       </c>
       <c r="O23" s="256" t="s">
-        <v>651</v>
+        <v>590</v>
       </c>
     </row>
     <row r="24" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I24" s="257" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>77</v>
@@ -18089,10 +18092,10 @@
         <v>388</v>
       </c>
       <c r="N24" s="256" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="O24" s="256" t="s">
-        <v>907</v>
+        <v>651</v>
       </c>
     </row>
     <row r="25" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18109,7 +18112,7 @@
         <v>506</v>
       </c>
       <c r="O25" s="256" t="s">
-        <v>591</v>
+        <v>906</v>
       </c>
     </row>
     <row r="26" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18126,7 +18129,7 @@
         <v>507</v>
       </c>
       <c r="O26" s="256" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="27" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18143,12 +18146,12 @@
         <v>508</v>
       </c>
       <c r="O27" s="256" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="28" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I28" s="257" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>81</v>
@@ -18174,27 +18177,27 @@
         <v>393</v>
       </c>
       <c r="N29" s="256" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="O29" s="256" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="30" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I30" s="257" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>83</v>
       </c>
       <c r="M30" s="256" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="N30" s="256" t="s">
         <v>510</v>
       </c>
       <c r="O30" s="256" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="31" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18211,10 +18214,10 @@
         <v>511</v>
       </c>
       <c r="O31" s="256" t="s">
-        <v>652</v>
-      </c>
-    </row>
-    <row r="32" spans="9:20" s="1" customFormat="1" ht="27" thickBot="1">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="32" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I32" s="258" t="s">
         <v>213</v>
       </c>
@@ -18225,13 +18228,13 @@
         <v>395</v>
       </c>
       <c r="N32" s="256" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="O32" s="256" t="s">
-        <v>596</v>
-      </c>
-    </row>
-    <row r="33" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="33" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I33" s="258" t="s">
         <v>214</v>
       </c>
@@ -18245,7 +18248,7 @@
         <v>512</v>
       </c>
       <c r="O33" s="256" t="s">
-        <v>908</v>
+        <v>596</v>
       </c>
     </row>
     <row r="34" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18262,10 +18265,10 @@
         <v>513</v>
       </c>
       <c r="O34" s="256" t="s">
-        <v>653</v>
-      </c>
-    </row>
-    <row r="35" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
+        <v>907</v>
+      </c>
+    </row>
+    <row r="35" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I35" s="258" t="s">
         <v>233</v>
       </c>
@@ -18279,10 +18282,10 @@
         <v>514</v>
       </c>
       <c r="O35" s="256" t="s">
-        <v>597</v>
-      </c>
-    </row>
-    <row r="36" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+        <v>653</v>
+      </c>
+    </row>
+    <row r="36" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I36" s="258" t="s">
         <v>216</v>
       </c>
@@ -18296,7 +18299,7 @@
         <v>515</v>
       </c>
       <c r="O36" s="256" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="37" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18307,13 +18310,13 @@
         <v>86</v>
       </c>
       <c r="M37" s="256" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="N37" s="256" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="O37" s="256" t="s">
-        <v>909</v>
+        <v>598</v>
       </c>
     </row>
     <row r="38" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18330,7 +18333,7 @@
         <v>516</v>
       </c>
       <c r="O38" s="256" t="s">
-        <v>599</v>
+        <v>908</v>
       </c>
     </row>
     <row r="39" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18347,7 +18350,7 @@
         <v>517</v>
       </c>
       <c r="O39" s="256" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="40" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18361,7 +18364,7 @@
         <v>518</v>
       </c>
       <c r="O40" s="256" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="41" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18369,13 +18372,13 @@
         <v>221</v>
       </c>
       <c r="M41" s="256" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="N41" s="256" t="s">
         <v>519</v>
       </c>
       <c r="O41" s="256" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="42" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18389,7 +18392,7 @@
         <v>520</v>
       </c>
       <c r="O42" s="256" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="43" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18403,10 +18406,10 @@
         <v>521</v>
       </c>
       <c r="O43" s="256" t="s">
-        <v>604</v>
-      </c>
-    </row>
-    <row r="44" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="44" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I44" s="258" t="s">
         <v>228</v>
       </c>
@@ -18417,10 +18420,10 @@
         <v>522</v>
       </c>
       <c r="O44" s="256" t="s">
-        <v>605</v>
-      </c>
-    </row>
-    <row r="45" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="45" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I45" s="258" t="s">
         <v>229</v>
       </c>
@@ -18431,7 +18434,7 @@
         <v>523</v>
       </c>
       <c r="O45" s="256" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="46" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18445,7 +18448,7 @@
         <v>524</v>
       </c>
       <c r="O46" s="256" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="47" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18459,7 +18462,7 @@
         <v>525</v>
       </c>
       <c r="O47" s="256" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="48" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18473,7 +18476,7 @@
         <v>526</v>
       </c>
       <c r="O48" s="256" t="s">
-        <v>910</v>
+        <v>608</v>
       </c>
     </row>
     <row r="49" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18487,7 +18490,7 @@
         <v>527</v>
       </c>
       <c r="O49" s="256" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
     </row>
     <row r="50" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18501,7 +18504,7 @@
         <v>528</v>
       </c>
       <c r="O50" s="256" t="s">
-        <v>609</v>
+        <v>910</v>
       </c>
     </row>
     <row r="51" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18512,7 +18515,7 @@
         <v>529</v>
       </c>
       <c r="O51" s="256" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="52" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18520,10 +18523,10 @@
         <v>413</v>
       </c>
       <c r="N52" s="256" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="O52" s="256" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="53" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
@@ -18534,7 +18537,7 @@
         <v>573</v>
       </c>
       <c r="O53" s="256" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="54" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18545,29 +18548,29 @@
         <v>530</v>
       </c>
       <c r="O54" s="256" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="55" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M55" s="256" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="N55" s="256" t="s">
         <v>531</v>
       </c>
       <c r="O55" s="256" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="56" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M56" s="256" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="N56" s="256" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="O56" s="256" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="57" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18578,7 +18581,7 @@
         <v>532</v>
       </c>
       <c r="O57" s="256" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="58" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18589,7 +18592,7 @@
         <v>533</v>
       </c>
       <c r="O58" s="256" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="59" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18600,7 +18603,7 @@
         <v>534</v>
       </c>
       <c r="O59" s="256" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="60" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18611,7 +18614,7 @@
         <v>535</v>
       </c>
       <c r="O60" s="256" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="61" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18622,7 +18625,7 @@
         <v>536</v>
       </c>
       <c r="O61" s="256" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="62" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18633,18 +18636,18 @@
         <v>538</v>
       </c>
       <c r="O62" s="256" t="s">
-        <v>621</v>
-      </c>
-    </row>
-    <row r="63" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="63" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M63" s="256" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="N63" s="256" t="s">
         <v>539</v>
       </c>
       <c r="O63" s="256" t="s">
-        <v>654</v>
+        <v>621</v>
       </c>
     </row>
     <row r="64" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
@@ -18655,29 +18658,29 @@
         <v>540</v>
       </c>
       <c r="O64" s="256" t="s">
-        <v>622</v>
-      </c>
-    </row>
-    <row r="65" spans="13:20" s="1" customFormat="1" ht="27" thickBot="1">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="65" spans="13:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M65" s="256" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="N65" s="256" t="s">
         <v>541</v>
       </c>
       <c r="O65" s="256" t="s">
-        <v>912</v>
-      </c>
-    </row>
-    <row r="66" spans="13:20" s="1" customFormat="1" ht="15.75" thickBot="1">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="66" spans="13:20" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M66" s="256" t="s">
         <v>423</v>
       </c>
       <c r="N66" s="256" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="O66" s="256" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
     </row>
     <row r="67" spans="13:20" ht="15.75" thickBot="1">
@@ -18685,10 +18688,10 @@
         <v>424</v>
       </c>
       <c r="N67" s="256" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="O67" s="256" t="s">
-        <v>623</v>
+        <v>912</v>
       </c>
       <c r="P67" s="1"/>
       <c r="Q67" s="1"/>
@@ -18696,7 +18699,7 @@
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
     </row>
-    <row r="68" spans="13:20" ht="27" thickBot="1">
+    <row r="68" spans="13:20" ht="15.75" thickBot="1">
       <c r="M68" s="256" t="s">
         <v>425</v>
       </c>
@@ -18704,29 +18707,29 @@
         <v>542</v>
       </c>
       <c r="O68" s="256" t="s">
-        <v>624</v>
-      </c>
-    </row>
-    <row r="69" spans="13:20" ht="15.75" thickBot="1">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="69" spans="13:20" ht="27" thickBot="1">
       <c r="M69" s="256" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="N69" s="256" t="s">
         <v>543</v>
       </c>
       <c r="O69" s="256" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="70" spans="13:20" ht="15.75" thickBot="1">
       <c r="M70" s="256" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="N70" s="256" t="s">
         <v>544</v>
       </c>
       <c r="O70" s="256" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="71" spans="13:20" ht="15.75" thickBot="1">
@@ -18734,10 +18737,10 @@
         <v>426</v>
       </c>
       <c r="N71" s="256" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="O71" s="256" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="72" spans="13:20" ht="15.75" thickBot="1">
@@ -18748,7 +18751,7 @@
         <v>545</v>
       </c>
       <c r="O72" s="256" t="s">
-        <v>914</v>
+        <v>627</v>
       </c>
     </row>
     <row r="73" spans="13:20" ht="27" thickBot="1">
@@ -18759,7 +18762,7 @@
         <v>546</v>
       </c>
       <c r="O73" s="256" t="s">
-        <v>628</v>
+        <v>913</v>
       </c>
     </row>
     <row r="74" spans="13:20" ht="15.75" thickBot="1">
@@ -18770,18 +18773,18 @@
         <v>547</v>
       </c>
       <c r="O74" s="256" t="s">
-        <v>916</v>
+        <v>628</v>
       </c>
     </row>
     <row r="75" spans="13:20" ht="15.75" thickBot="1">
       <c r="M75" s="256" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="N75" s="256" t="s">
         <v>548</v>
       </c>
       <c r="O75" s="256" t="s">
-        <v>629</v>
+        <v>915</v>
       </c>
     </row>
     <row r="76" spans="13:20" ht="15.75" thickBot="1">
@@ -18792,7 +18795,7 @@
         <v>549</v>
       </c>
       <c r="O76" s="256" t="s">
-        <v>917</v>
+        <v>629</v>
       </c>
     </row>
     <row r="77" spans="13:20" ht="15.75" thickBot="1">
@@ -18803,7 +18806,7 @@
         <v>550</v>
       </c>
       <c r="O77" s="256" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
     </row>
     <row r="78" spans="13:20" ht="15.75" thickBot="1">
@@ -18814,7 +18817,7 @@
         <v>551</v>
       </c>
       <c r="O78" s="256" t="s">
-        <v>630</v>
+        <v>917</v>
       </c>
     </row>
     <row r="79" spans="13:20" ht="27" thickBot="1">
@@ -18825,7 +18828,7 @@
         <v>552</v>
       </c>
       <c r="O79" s="256" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="80" spans="13:20" ht="15.75" thickBot="1">
@@ -18833,10 +18836,10 @@
         <v>434</v>
       </c>
       <c r="N80" s="256" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="O80" s="256" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="81" spans="13:15" ht="15.75" thickBot="1">
@@ -18847,7 +18850,7 @@
         <v>553</v>
       </c>
       <c r="O81" s="256" t="s">
-        <v>655</v>
+        <v>632</v>
       </c>
     </row>
     <row r="82" spans="13:15" ht="15.75" thickBot="1">
@@ -18858,7 +18861,7 @@
         <v>554</v>
       </c>
       <c r="O82" s="256" t="s">
-        <v>919</v>
+        <v>655</v>
       </c>
     </row>
     <row r="83" spans="13:15" ht="15.75" thickBot="1">
@@ -18866,10 +18869,10 @@
         <v>437</v>
       </c>
       <c r="N83" s="256" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="O83" s="256" t="s">
-        <v>633</v>
+        <v>918</v>
       </c>
     </row>
     <row r="84" spans="13:15" ht="15.75" thickBot="1">
@@ -18880,7 +18883,7 @@
         <v>555</v>
       </c>
       <c r="O84" s="256" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="85" spans="13:15" ht="15.75" thickBot="1">
@@ -18891,7 +18894,7 @@
         <v>556</v>
       </c>
       <c r="O85" s="256" t="s">
-        <v>635</v>
+        <v>634</v>
       </c>
     </row>
     <row r="86" spans="13:15" ht="15.75" thickBot="1">
@@ -18902,7 +18905,7 @@
         <v>557</v>
       </c>
       <c r="O86" s="256" t="s">
-        <v>636</v>
+        <v>635</v>
       </c>
     </row>
     <row r="87" spans="13:15" ht="15.75" thickBot="1">
@@ -18913,7 +18916,7 @@
         <v>558</v>
       </c>
       <c r="O87" s="256" t="s">
-        <v>637</v>
+        <v>636</v>
       </c>
     </row>
     <row r="88" spans="13:15" ht="15.75" thickBot="1">
@@ -18924,7 +18927,7 @@
         <v>559</v>
       </c>
       <c r="O88" s="256" t="s">
-        <v>921</v>
+        <v>637</v>
       </c>
     </row>
     <row r="89" spans="13:15" ht="15.75" thickBot="1">
@@ -18943,10 +18946,10 @@
         <v>444</v>
       </c>
       <c r="N90" s="256" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="O90" s="256" t="s">
-        <v>915</v>
+        <v>919</v>
       </c>
     </row>
     <row r="91" spans="13:15" ht="15.75" thickBot="1">
@@ -18957,7 +18960,7 @@
         <v>561</v>
       </c>
       <c r="O91" s="256" t="s">
-        <v>638</v>
+        <v>914</v>
       </c>
     </row>
     <row r="92" spans="13:15" ht="15.75" thickBot="1">
@@ -18968,18 +18971,18 @@
         <v>562</v>
       </c>
       <c r="O92" s="256" t="s">
-        <v>639</v>
+        <v>638</v>
       </c>
     </row>
     <row r="93" spans="13:15" ht="15.75" thickBot="1">
       <c r="M93" s="256" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="N93" s="256" t="s">
         <v>563</v>
       </c>
       <c r="O93" s="256" t="s">
-        <v>640</v>
+        <v>639</v>
       </c>
     </row>
     <row r="94" spans="13:15" ht="15.75" thickBot="1">
@@ -18990,7 +18993,7 @@
         <v>564</v>
       </c>
       <c r="O94" s="256" t="s">
-        <v>641</v>
+        <v>640</v>
       </c>
     </row>
     <row r="95" spans="13:15" ht="15.75" thickBot="1">
@@ -19001,7 +19004,7 @@
         <v>565</v>
       </c>
       <c r="O95" s="256" t="s">
-        <v>642</v>
+        <v>641</v>
       </c>
     </row>
     <row r="96" spans="13:15" ht="15.75" thickBot="1">
@@ -19012,7 +19015,7 @@
         <v>566</v>
       </c>
       <c r="O96" s="256" t="s">
-        <v>656</v>
+        <v>642</v>
       </c>
     </row>
     <row r="97" spans="13:15" ht="15.75" thickBot="1">
@@ -19023,7 +19026,7 @@
         <v>567</v>
       </c>
       <c r="O97" s="256" t="s">
-        <v>657</v>
+        <v>656</v>
       </c>
     </row>
     <row r="98" spans="13:15" ht="15.75" thickBot="1">
@@ -19034,7 +19037,7 @@
         <v>568</v>
       </c>
       <c r="O98" s="256" t="s">
-        <v>643</v>
+        <v>657</v>
       </c>
     </row>
     <row r="99" spans="13:15" ht="15.75" thickBot="1">
@@ -19045,7 +19048,7 @@
         <v>569</v>
       </c>
       <c r="O99" s="256" t="s">
-        <v>644</v>
+        <v>643</v>
       </c>
     </row>
     <row r="100" spans="13:15" ht="15.75" thickBot="1">
@@ -19056,7 +19059,7 @@
         <v>570</v>
       </c>
       <c r="O100" s="256" t="s">
-        <v>922</v>
+        <v>644</v>
       </c>
     </row>
     <row r="101" spans="13:15" ht="15.75" thickBot="1">
@@ -19067,7 +19070,7 @@
         <v>571</v>
       </c>
       <c r="O101" s="256" t="s">
-        <v>645</v>
+        <v>921</v>
       </c>
     </row>
     <row r="102" spans="13:15" ht="15.75" thickBot="1">
@@ -19078,7 +19081,7 @@
         <v>572</v>
       </c>
       <c r="O102" s="256" t="s">
-        <v>923</v>
+        <v>645</v>
       </c>
     </row>
     <row r="103" spans="13:15" ht="27" thickBot="1">
@@ -19089,7 +19092,7 @@
         <v>573</v>
       </c>
       <c r="O103" s="256" t="s">
-        <v>646</v>
+        <v>922</v>
       </c>
     </row>
     <row r="104" spans="13:15" ht="15.75" thickBot="1">
@@ -19097,7 +19100,7 @@
         <v>456</v>
       </c>
       <c r="O104" s="256" t="s">
-        <v>647</v>
+        <v>646</v>
       </c>
     </row>
     <row r="105" spans="13:15" ht="15.75" thickBot="1">
@@ -19105,7 +19108,7 @@
         <v>458</v>
       </c>
       <c r="O105" s="256" t="s">
-        <v>648</v>
+        <v>647</v>
       </c>
     </row>
     <row r="106" spans="13:15" ht="15.75" thickBot="1">
@@ -19113,30 +19116,33 @@
         <v>459</v>
       </c>
       <c r="O106" s="256" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="107" spans="13:15" ht="27" thickBot="1">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="107" spans="13:15" ht="15.75" thickBot="1">
       <c r="M107" s="256" t="s">
         <v>460</v>
       </c>
       <c r="O107" s="256" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="108" spans="13:15" ht="15.75" thickBot="1">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="108" spans="13:15" ht="27" thickBot="1">
       <c r="M108" s="256" t="s">
         <v>461</v>
       </c>
+      <c r="O108" s="256" t="s">
+        <v>658</v>
+      </c>
     </row>
     <row r="109" spans="13:15" ht="15.75" thickBot="1">
       <c r="M109" s="256" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
     </row>
     <row r="110" spans="13:15" ht="15.75" thickBot="1">
       <c r="M110" s="256" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
     </row>
     <row r="111" spans="13:15" ht="15.75" thickBot="1">
@@ -19206,7 +19212,7 @@
     </row>
     <row r="124" spans="13:13" ht="15.75" thickBot="1">
       <c r="M124" s="256" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
     </row>
     <row r="125" spans="13:13" ht="15.75" thickBot="1">
@@ -19216,7 +19222,7 @@
     </row>
     <row r="126" spans="13:13" ht="15.75" thickBot="1">
       <c r="M126" s="256" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
     </row>
     <row r="127" spans="13:13" ht="15.75" thickBot="1">
@@ -19241,7 +19247,7 @@
     </row>
     <row r="131" spans="13:13" ht="15.75" thickBot="1">
       <c r="M131" s="256" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
     </row>
     <row r="132" spans="13:13" ht="15.75" thickBot="1">

</xml_diff>

<commit_message>
Split greenhouses cultivation_types in two between heated and not
</commit_message>
<xml_diff>
--- a/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
+++ b/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1005" windowWidth="24240" windowHeight="13680" tabRatio="463"/>
+    <workbookView xWindow="120" yWindow="1005" windowWidth="24240" windowHeight="13680" tabRatio="463" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="127" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2319" uniqueCount="1058">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="1060">
   <si>
     <t>Country</t>
   </si>
@@ -3300,12 +3300,6 @@
     <t>open ground</t>
   </si>
   <si>
-    <t>greenhouse, open ground</t>
-  </si>
-  <si>
-    <t>greenhouse, hydroponic system</t>
-  </si>
-  <si>
     <t>Lifetime of orchard</t>
   </si>
   <si>
@@ -3496,6 +3490,18 @@
   </si>
   <si>
     <t>Snow winter dry cold summer</t>
+  </si>
+  <si>
+    <t>greenhouse, open ground, heated</t>
+  </si>
+  <si>
+    <t>greenhouse, open ground, unheated</t>
+  </si>
+  <si>
+    <t>greenhouse, hydroponic system, unheated</t>
+  </si>
+  <si>
+    <t>greenhouse, hydroponic system, heated</t>
   </si>
 </sst>
 </file>
@@ -8303,7 +8309,7 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
@@ -8377,7 +8383,7 @@
     <row r="6" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A6" s="154"/>
       <c r="B6" s="266" t="s">
-        <v>1045</v>
+        <v>1043</v>
       </c>
       <c r="C6" s="267"/>
       <c r="D6" s="267"/>
@@ -12815,7 +12821,7 @@
   </sheetPr>
   <dimension ref="A1:AB225"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
       <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
@@ -12837,7 +12843,7 @@
   <sheetData>
     <row r="1" spans="1:8" hidden="1">
       <c r="A1" s="98" t="s">
-        <v>1044</v>
+        <v>1042</v>
       </c>
       <c r="C1" s="100" t="s">
         <v>236</v>
@@ -13272,7 +13278,7 @@
       <c r="D28" s="20" t="s">
         <v>980</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="108" t="s">
         <v>99</v>
       </c>
       <c r="F28" s="21"/>
@@ -13474,11 +13480,11 @@
     </row>
     <row r="41" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A41" s="252" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="B41" s="12"/>
       <c r="C41" s="26" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="D41" s="7" t="s">
         <v>28</v>
@@ -13774,7 +13780,7 @@
     </row>
     <row r="59" spans="1:8" outlineLevel="1">
       <c r="C59" s="41" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="D59" s="7"/>
       <c r="E59" s="108"/>
@@ -13788,7 +13794,7 @@
       </c>
       <c r="B60" s="12"/>
       <c r="C60" s="46" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="D60" s="7" t="s">
         <v>31</v>
@@ -13803,7 +13809,7 @@
     <row r="61" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="B61" s="12"/>
       <c r="C61" s="41" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="D61" s="7"/>
       <c r="E61" s="108"/>
@@ -13813,11 +13819,11 @@
     </row>
     <row r="62" spans="1:8" s="252" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A62" s="252" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="B62" s="12"/>
       <c r="C62" s="46" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="D62" s="7" t="s">
         <v>31</v>
@@ -13831,11 +13837,11 @@
     </row>
     <row r="63" spans="1:8" s="252" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A63" s="252" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="B63" s="12"/>
       <c r="C63" s="46" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="D63" s="7" t="s">
         <v>31</v>
@@ -13849,11 +13855,11 @@
     </row>
     <row r="64" spans="1:8" s="252" customFormat="1" ht="15" customHeight="1" outlineLevel="1">
       <c r="A64" s="252" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="B64" s="12"/>
       <c r="C64" s="46" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="D64" s="7" t="s">
         <v>31</v>
@@ -14352,7 +14358,7 @@
     <row r="93" spans="1:8" ht="21">
       <c r="B93" s="70"/>
       <c r="C93" s="71" t="s">
-        <v>1047</v>
+        <v>1045</v>
       </c>
       <c r="D93" s="72" t="s">
         <v>8</v>
@@ -14472,14 +14478,14 @@
     </row>
     <row r="100" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A100" s="252" t="s">
-        <v>1010</v>
+        <v>1008</v>
       </c>
       <c r="B100" s="12"/>
       <c r="C100" s="30" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="D100" s="7" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="E100" s="109" t="s">
         <v>99</v>
@@ -14490,11 +14496,11 @@
     </row>
     <row r="101" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A101" s="252" t="s">
-        <v>1011</v>
+        <v>1009</v>
       </c>
       <c r="B101" s="12"/>
       <c r="C101" s="46" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="D101" s="39" t="s">
         <v>22</v>
@@ -14508,11 +14514,11 @@
     </row>
     <row r="102" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A102" s="252" t="s">
-        <v>1012</v>
+        <v>1010</v>
       </c>
       <c r="B102" s="12"/>
       <c r="C102" s="46" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="D102" s="39" t="s">
         <v>22</v>
@@ -14526,11 +14532,11 @@
     </row>
     <row r="103" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A103" s="252" t="s">
-        <v>1013</v>
+        <v>1011</v>
       </c>
       <c r="B103" s="12"/>
       <c r="C103" s="46" t="s">
-        <v>1009</v>
+        <v>1007</v>
       </c>
       <c r="D103" s="39" t="s">
         <v>22</v>
@@ -14545,7 +14551,7 @@
     <row r="104" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="B104" s="12"/>
       <c r="C104" s="30" t="s">
-        <v>1014</v>
+        <v>1012</v>
       </c>
       <c r="D104" s="7"/>
       <c r="E104" s="109"/>
@@ -14555,16 +14561,16 @@
     </row>
     <row r="105" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A105" s="252" t="s">
-        <v>1021</v>
+        <v>1019</v>
       </c>
       <c r="B105" s="12"/>
       <c r="C105" s="46" t="s">
-        <v>1015</v>
+        <v>1013</v>
       </c>
       <c r="D105" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E105" s="22" t="s">
+      <c r="E105" s="109" t="s">
         <v>99</v>
       </c>
       <c r="F105" s="24"/>
@@ -14573,16 +14579,16 @@
     </row>
     <row r="106" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A106" s="252" t="s">
-        <v>1022</v>
+        <v>1020</v>
       </c>
       <c r="B106" s="12"/>
       <c r="C106" s="46" t="s">
-        <v>1016</v>
+        <v>1014</v>
       </c>
       <c r="D106" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E106" s="22" t="s">
+      <c r="E106" s="109" t="s">
         <v>99</v>
       </c>
       <c r="F106" s="24"/>
@@ -14591,16 +14597,16 @@
     </row>
     <row r="107" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A107" s="252" t="s">
-        <v>1023</v>
+        <v>1021</v>
       </c>
       <c r="B107" s="12"/>
       <c r="C107" s="46" t="s">
-        <v>1017</v>
+        <v>1015</v>
       </c>
       <c r="D107" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E107" s="22" t="s">
+      <c r="E107" s="109" t="s">
         <v>99</v>
       </c>
       <c r="F107" s="24"/>
@@ -14609,16 +14615,16 @@
     </row>
     <row r="108" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A108" s="252" t="s">
-        <v>1024</v>
+        <v>1022</v>
       </c>
       <c r="B108" s="12"/>
       <c r="C108" s="46" t="s">
-        <v>1018</v>
+        <v>1016</v>
       </c>
       <c r="D108" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E108" s="22" t="s">
+      <c r="E108" s="109" t="s">
         <v>99</v>
       </c>
       <c r="F108" s="24"/>
@@ -14627,16 +14633,16 @@
     </row>
     <row r="109" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A109" s="252" t="s">
-        <v>1025</v>
+        <v>1023</v>
       </c>
       <c r="B109" s="12"/>
       <c r="C109" s="46" t="s">
-        <v>1019</v>
+        <v>1017</v>
       </c>
       <c r="D109" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E109" s="22" t="s">
+      <c r="E109" s="109" t="s">
         <v>99</v>
       </c>
       <c r="F109" s="24"/>
@@ -14645,16 +14651,16 @@
     </row>
     <row r="110" spans="1:8" s="252" customFormat="1" outlineLevel="1">
       <c r="A110" s="252" t="s">
-        <v>1026</v>
+        <v>1024</v>
       </c>
       <c r="B110" s="12"/>
       <c r="C110" s="46" t="s">
-        <v>1020</v>
+        <v>1018</v>
       </c>
       <c r="D110" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="E110" s="22" t="s">
+      <c r="E110" s="109" t="s">
         <v>99</v>
       </c>
       <c r="F110" s="24"/>
@@ -15405,7 +15411,7 @@
       </c>
       <c r="B156" s="7"/>
       <c r="C156" s="5" t="s">
-        <v>1027</v>
+        <v>1025</v>
       </c>
       <c r="D156" s="7" t="s">
         <v>27</v>
@@ -15447,7 +15453,7 @@
       </c>
       <c r="B158" s="12"/>
       <c r="C158" s="29" t="s">
-        <v>1028</v>
+        <v>1026</v>
       </c>
       <c r="D158" s="12" t="s">
         <v>27</v>
@@ -15532,7 +15538,7 @@
       </c>
       <c r="B162" s="12"/>
       <c r="C162" s="29" t="s">
-        <v>1029</v>
+        <v>1027</v>
       </c>
       <c r="D162" s="12" t="s">
         <v>27</v>
@@ -15617,7 +15623,7 @@
       </c>
       <c r="B166" s="12"/>
       <c r="C166" s="134" t="s">
-        <v>1030</v>
+        <v>1028</v>
       </c>
       <c r="D166" s="139" t="s">
         <v>27</v>
@@ -15702,7 +15708,7 @@
       </c>
       <c r="B170" s="12"/>
       <c r="C170" s="29" t="s">
-        <v>1031</v>
+        <v>1029</v>
       </c>
       <c r="D170" s="12" t="s">
         <v>27</v>
@@ -15788,7 +15794,7 @@
       </c>
       <c r="B174" s="12"/>
       <c r="C174" s="134" t="s">
-        <v>1032</v>
+        <v>1030</v>
       </c>
       <c r="D174" s="12" t="s">
         <v>27</v>
@@ -15874,7 +15880,7 @@
       </c>
       <c r="B178" s="12"/>
       <c r="C178" s="134" t="s">
-        <v>1033</v>
+        <v>1031</v>
       </c>
       <c r="D178" s="139" t="s">
         <v>27</v>
@@ -15937,7 +15943,7 @@
       </c>
       <c r="B181" s="117"/>
       <c r="C181" s="117" t="s">
-        <v>1034</v>
+        <v>1032</v>
       </c>
       <c r="D181" s="118" t="s">
         <v>8</v>
@@ -15955,11 +15961,11 @@
     </row>
     <row r="182" spans="1:28" s="253" customFormat="1" ht="14.1" customHeight="1" outlineLevel="1">
       <c r="A182" s="253" t="s">
-        <v>1035</v>
+        <v>1033</v>
       </c>
       <c r="B182" s="12"/>
       <c r="C182" s="134" t="s">
-        <v>1036</v>
+        <v>1034</v>
       </c>
       <c r="D182" s="139" t="s">
         <v>27</v>
@@ -16781,11 +16787,11 @@
     </row>
     <row r="212" spans="1:28" outlineLevel="1">
       <c r="A212" s="4" t="s">
-        <v>1039</v>
+        <v>1037</v>
       </c>
       <c r="B212" s="7"/>
       <c r="C212" s="26" t="s">
-        <v>1037</v>
+        <v>1035</v>
       </c>
       <c r="D212" s="7" t="s">
         <v>90</v>
@@ -16799,11 +16805,11 @@
     </row>
     <row r="213" spans="1:28" outlineLevel="1">
       <c r="A213" s="4" t="s">
-        <v>1040</v>
+        <v>1038</v>
       </c>
       <c r="B213" s="7"/>
       <c r="C213" s="26" t="s">
-        <v>1038</v>
+        <v>1036</v>
       </c>
       <c r="D213" s="7" t="s">
         <v>90</v>
@@ -16924,11 +16930,11 @@
     </row>
     <row r="218" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A218" s="11" t="s">
-        <v>1048</v>
+        <v>1046</v>
       </c>
       <c r="B218" s="12"/>
       <c r="C218" s="26" t="s">
-        <v>1041</v>
+        <v>1039</v>
       </c>
       <c r="D218" s="86" t="s">
         <v>27</v>
@@ -16947,7 +16953,7 @@
     </row>
     <row r="219" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A219" s="11" t="s">
-        <v>1049</v>
+        <v>1047</v>
       </c>
       <c r="B219" s="12"/>
       <c r="C219" s="150" t="s">
@@ -16970,16 +16976,16 @@
     </row>
     <row r="220" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A220" s="11" t="s">
-        <v>1050</v>
+        <v>1048</v>
       </c>
       <c r="B220" s="12"/>
       <c r="C220" s="150" t="s">
-        <v>1042</v>
+        <v>1040</v>
       </c>
       <c r="D220" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="E220" s="251" t="s">
+      <c r="E220" s="249" t="s">
         <v>99</v>
       </c>
       <c r="F220" s="51"/>
@@ -16993,11 +16999,11 @@
     </row>
     <row r="221" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A221" s="11" t="s">
-        <v>1051</v>
+        <v>1049</v>
       </c>
       <c r="B221" s="12"/>
       <c r="C221" s="150" t="s">
-        <v>1043</v>
+        <v>1041</v>
       </c>
       <c r="D221" s="86" t="s">
         <v>22</v>
@@ -17016,7 +17022,7 @@
     </row>
     <row r="222" spans="1:28" s="253" customFormat="1" outlineLevel="1">
       <c r="A222" s="11" t="s">
-        <v>1052</v>
+        <v>1050</v>
       </c>
       <c r="B222" s="12"/>
       <c r="C222" s="150" t="s">
@@ -17220,7 +17226,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$U$2:$U$4</xm:f>
+            <xm:f>Lists!$U$2:$U$6</xm:f>
           </x14:formula1>
           <xm:sqref>E30</xm:sqref>
         </x14:dataValidation>
@@ -17249,10 +17255,10 @@
   </sheetPr>
   <dimension ref="A1:V141"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B35" sqref="B35"/>
-      <selection pane="bottomLeft" activeCell="R22" sqref="R22"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17460,7 +17466,7 @@
         <v/>
       </c>
       <c r="U3" s="1" t="s">
-        <v>992</v>
+        <v>1057</v>
       </c>
       <c r="V3" s="258" t="s">
         <v>990</v>
@@ -17528,8 +17534,8 @@
         <f t="shared" ref="T4:T22" si="0">IF(T$1=P$3,Q4,IF(T$1=P$4,R4,IF(T$1=P$5,S4,"")))</f>
         <v/>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>993</v>
+      <c r="U4" s="258" t="s">
+        <v>1056</v>
       </c>
     </row>
     <row r="5" spans="1:22" s="1" customFormat="1" ht="27" thickBot="1">
@@ -17594,6 +17600,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="U5" s="258" t="s">
+        <v>1058</v>
+      </c>
     </row>
     <row r="6" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="A6" s="1" t="s">
@@ -17648,6 +17657,9 @@
         <f t="shared" si="0"/>
         <v/>
       </c>
+      <c r="U6" s="258" t="s">
+        <v>1059</v>
+      </c>
     </row>
     <row r="7" spans="1:22" s="1" customFormat="1" ht="52.5" thickBot="1">
       <c r="A7" s="1" t="s">
@@ -17687,7 +17699,7 @@
         <v>578</v>
       </c>
       <c r="Q7" s="259" t="s">
-        <v>1053</v>
+        <v>1051</v>
       </c>
       <c r="R7" s="1" t="s">
         <v>960</v>
@@ -17861,7 +17873,7 @@
         <v>582</v>
       </c>
       <c r="R12" s="258" t="s">
-        <v>1054</v>
+        <v>1052</v>
       </c>
       <c r="T12" s="258" t="str">
         <f t="shared" si="0"/>
@@ -17984,7 +17996,7 @@
         <v>500</v>
       </c>
       <c r="O17" s="256" t="s">
-        <v>1046</v>
+        <v>1044</v>
       </c>
       <c r="R17" s="258" t="s">
         <v>970</v>
@@ -18035,7 +18047,7 @@
         <v>586</v>
       </c>
       <c r="R19" s="258" t="s">
-        <v>1055</v>
+        <v>1053</v>
       </c>
       <c r="T19" s="258" t="str">
         <f t="shared" si="0"/>
@@ -18059,7 +18071,7 @@
         <v>587</v>
       </c>
       <c r="R20" s="258" t="s">
-        <v>1056</v>
+        <v>1054</v>
       </c>
       <c r="T20" s="258" t="str">
         <f t="shared" si="0"/>
@@ -18083,7 +18095,7 @@
         <v>588</v>
       </c>
       <c r="R21" s="258" t="s">
-        <v>1057</v>
+        <v>1055</v>
       </c>
       <c r="T21" s="258" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Finish addition of MA,CS and berries
</commit_message>
<xml_diff>
--- a/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
+++ b/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1005" windowWidth="24240" windowHeight="13680" tabRatio="463" activeTab="2"/>
+    <workbookView xWindow="120" yWindow="1005" windowWidth="24240" windowHeight="13680" tabRatio="463"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="127" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2321" uniqueCount="1060">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2326" uniqueCount="1065">
   <si>
     <t>Country</t>
   </si>
@@ -3502,6 +3502,21 @@
   </si>
   <si>
     <t>greenhouse, hydroponic system, heated</t>
+  </si>
+  <si>
+    <t>Serbia</t>
+  </si>
+  <si>
+    <t>Morocco</t>
+  </si>
+  <si>
+    <t>Blueberry</t>
+  </si>
+  <si>
+    <t>Cranberry</t>
+  </si>
+  <si>
+    <t>Raspberry</t>
   </si>
 </sst>
 </file>
@@ -6132,6 +6147,21 @@
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="84" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -6143,21 +6173,6 @@
     </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="84" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="50" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -8309,7 +8324,7 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
@@ -8371,25 +8386,25 @@
     </row>
     <row r="5" spans="1:9" s="160" customFormat="1" ht="54.75" customHeight="1">
       <c r="A5" s="159"/>
-      <c r="B5" s="265"/>
-      <c r="C5" s="265"/>
-      <c r="D5" s="265"/>
-      <c r="E5" s="265"/>
-      <c r="F5" s="265"/>
-      <c r="G5" s="265"/>
+      <c r="B5" s="261"/>
+      <c r="C5" s="261"/>
+      <c r="D5" s="261"/>
+      <c r="E5" s="261"/>
+      <c r="F5" s="261"/>
+      <c r="G5" s="261"/>
       <c r="H5" s="156"/>
       <c r="I5" s="156"/>
     </row>
     <row r="6" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A6" s="154"/>
-      <c r="B6" s="266" t="s">
+      <c r="B6" s="262" t="s">
         <v>1043</v>
       </c>
-      <c r="C6" s="267"/>
-      <c r="D6" s="267"/>
-      <c r="E6" s="267"/>
-      <c r="F6" s="267"/>
-      <c r="G6" s="267"/>
+      <c r="C6" s="263"/>
+      <c r="D6" s="263"/>
+      <c r="E6" s="263"/>
+      <c r="F6" s="263"/>
+      <c r="G6" s="263"/>
       <c r="H6" s="156"/>
       <c r="I6" s="156"/>
     </row>
@@ -8406,14 +8421,14 @@
     </row>
     <row r="8" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A8" s="154"/>
-      <c r="B8" s="268" t="s">
+      <c r="B8" s="264" t="s">
         <v>708</v>
       </c>
-      <c r="C8" s="268"/>
-      <c r="D8" s="268"/>
-      <c r="E8" s="268"/>
-      <c r="F8" s="268"/>
-      <c r="G8" s="268"/>
+      <c r="C8" s="264"/>
+      <c r="D8" s="264"/>
+      <c r="E8" s="264"/>
+      <c r="F8" s="264"/>
+      <c r="G8" s="264"/>
       <c r="H8" s="161"/>
       <c r="I8" s="156"/>
     </row>
@@ -8430,14 +8445,14 @@
     </row>
     <row r="10" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A10" s="154"/>
-      <c r="B10" s="269" t="s">
+      <c r="B10" s="265" t="s">
         <v>772</v>
       </c>
-      <c r="C10" s="269"/>
-      <c r="D10" s="269"/>
-      <c r="E10" s="269"/>
-      <c r="F10" s="269"/>
-      <c r="G10" s="269"/>
+      <c r="C10" s="265"/>
+      <c r="D10" s="265"/>
+      <c r="E10" s="265"/>
+      <c r="F10" s="265"/>
+      <c r="G10" s="265"/>
       <c r="H10" s="156"/>
       <c r="I10" s="156"/>
     </row>
@@ -8445,10 +8460,10 @@
       <c r="A11" s="154"/>
       <c r="B11" s="173"/>
       <c r="C11" s="173"/>
-      <c r="D11" s="269"/>
-      <c r="E11" s="269"/>
-      <c r="F11" s="269"/>
-      <c r="G11" s="269"/>
+      <c r="D11" s="265"/>
+      <c r="E11" s="265"/>
+      <c r="F11" s="265"/>
+      <c r="G11" s="265"/>
       <c r="H11" s="156"/>
       <c r="I11" s="156"/>
     </row>
@@ -8521,23 +8536,23 @@
     </row>
     <row r="17" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A17" s="154"/>
-      <c r="B17" s="262" t="s">
+      <c r="B17" s="267" t="s">
         <v>711</v>
       </c>
-      <c r="C17" s="262"/>
-      <c r="D17" s="262"/>
-      <c r="E17" s="262"/>
-      <c r="F17" s="262"/>
-      <c r="G17" s="262"/>
+      <c r="C17" s="267"/>
+      <c r="D17" s="267"/>
+      <c r="E17" s="267"/>
+      <c r="F17" s="267"/>
+      <c r="G17" s="267"/>
       <c r="H17" s="161"/>
       <c r="I17" s="156"/>
     </row>
     <row r="18" spans="1:9" s="160" customFormat="1">
       <c r="A18" s="159"/>
-      <c r="B18" s="263" t="s">
+      <c r="B18" s="268" t="s">
         <v>712</v>
       </c>
-      <c r="C18" s="263"/>
+      <c r="C18" s="268"/>
       <c r="D18" s="180" t="s">
         <v>713</v>
       </c>
@@ -8555,10 +8570,10 @@
     </row>
     <row r="19" spans="1:9" s="160" customFormat="1">
       <c r="A19" s="159"/>
-      <c r="B19" s="264" t="s">
+      <c r="B19" s="269" t="s">
         <v>717</v>
       </c>
-      <c r="C19" s="264"/>
+      <c r="C19" s="269"/>
       <c r="D19" s="166" t="s">
         <v>718</v>
       </c>
@@ -8597,10 +8612,10 @@
     </row>
     <row r="21" spans="1:9" s="160" customFormat="1">
       <c r="A21" s="159"/>
-      <c r="B21" s="261" t="s">
+      <c r="B21" s="266" t="s">
         <v>720</v>
       </c>
-      <c r="C21" s="261"/>
+      <c r="C21" s="266"/>
       <c r="D21" s="167" t="s">
         <v>721</v>
       </c>
@@ -8618,10 +8633,10 @@
     </row>
     <row r="22" spans="1:9" s="160" customFormat="1" ht="25.5">
       <c r="A22" s="159"/>
-      <c r="B22" s="261" t="s">
+      <c r="B22" s="266" t="s">
         <v>724</v>
       </c>
-      <c r="C22" s="261"/>
+      <c r="C22" s="266"/>
       <c r="D22" s="167" t="s">
         <v>725</v>
       </c>
@@ -8735,12 +8750,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="D11:G11"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="B21:C21"/>
@@ -8749,6 +8758,12 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D15:G15"/>
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <phoneticPr fontId="83" type="noConversion"/>
   <hyperlinks>
@@ -12821,10 +12836,10 @@
   </sheetPr>
   <dimension ref="A1:AB225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -17128,12 +17143,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="19">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$J$2:$J$39</xm:f>
-          </x14:formula1>
-          <xm:sqref>D5</xm:sqref>
-        </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$A$2:$A$8</xm:f>
@@ -17202,12 +17211,6 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$I$2:$I$50</xm:f>
-          </x14:formula1>
-          <xm:sqref>D4</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
             <xm:f>Lists!$M$2:$M$141</xm:f>
           </x14:formula1>
           <xm:sqref>C134:C136</xm:sqref>
@@ -17242,6 +17245,18 @@
           </x14:formula1>
           <xm:sqref>C148:C150</xm:sqref>
         </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$J$2:$J$41</xm:f>
+          </x14:formula1>
+          <xm:sqref>D5</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>Lists!$I$2:$I$53</xm:f>
+          </x14:formula1>
+          <xm:sqref>D4</xm:sqref>
+        </x14:dataValidation>
       </x14:dataValidations>
     </ext>
   </extLst>
@@ -17759,7 +17774,7 @@
         <v>199</v>
       </c>
       <c r="I9" s="257" t="s">
-        <v>926</v>
+        <v>1062</v>
       </c>
       <c r="J9" s="1" t="s">
         <v>61</v>
@@ -17791,8 +17806,8 @@
       <c r="G10" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="I10" s="258" t="s">
-        <v>197</v>
+      <c r="I10" s="257" t="s">
+        <v>926</v>
       </c>
       <c r="J10" s="1" t="s">
         <v>62</v>
@@ -17824,8 +17839,8 @@
       <c r="G11" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="I11" s="257" t="s">
-        <v>927</v>
+      <c r="I11" s="258" t="s">
+        <v>197</v>
       </c>
       <c r="J11" s="1" t="s">
         <v>63</v>
@@ -17858,7 +17873,7 @@
         <v>207</v>
       </c>
       <c r="I12" s="257" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="J12" s="1" t="s">
         <v>59</v>
@@ -17885,7 +17900,7 @@
         <v>208</v>
       </c>
       <c r="I13" s="257" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="J13" s="1" t="s">
         <v>65</v>
@@ -17911,8 +17926,8 @@
       <c r="G14" s="9" t="s">
         <v>865</v>
       </c>
-      <c r="I14" s="258" t="s">
-        <v>200</v>
+      <c r="I14" s="257" t="s">
+        <v>929</v>
       </c>
       <c r="J14" s="1" t="s">
         <v>67</v>
@@ -17936,7 +17951,7 @@
     </row>
     <row r="15" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I15" s="258" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J15" s="1" t="s">
         <v>68</v>
@@ -17960,7 +17975,7 @@
     </row>
     <row r="16" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I16" s="258" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>64</v>
@@ -17983,8 +17998,8 @@
       </c>
     </row>
     <row r="17" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I17" s="257" t="s">
-        <v>930</v>
+      <c r="I17" s="258" t="s">
+        <v>206</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>69</v>
@@ -18008,7 +18023,7 @@
     </row>
     <row r="18" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I18" s="257" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>70</v>
@@ -18032,7 +18047,7 @@
     </row>
     <row r="19" spans="9:20" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I19" s="257" t="s">
-        <v>932</v>
+        <v>1063</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>73</v>
@@ -18056,7 +18071,7 @@
     </row>
     <row r="20" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I20" s="257" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>71</v>
@@ -18080,7 +18095,7 @@
     </row>
     <row r="21" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I21" s="257" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>72</v>
@@ -18104,7 +18119,7 @@
     </row>
     <row r="22" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I22" s="257" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>74</v>
@@ -18127,8 +18142,8 @@
       </c>
     </row>
     <row r="23" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I23" s="258" t="s">
-        <v>231</v>
+      <c r="I23" s="257" t="s">
+        <v>934</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>75</v>
@@ -18145,10 +18160,10 @@
     </row>
     <row r="24" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I24" s="257" t="s">
-        <v>936</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>77</v>
+        <v>935</v>
+      </c>
+      <c r="J24" s="258" t="s">
+        <v>1061</v>
       </c>
       <c r="M24" s="256" t="s">
         <v>388</v>
@@ -18162,10 +18177,10 @@
     </row>
     <row r="25" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I25" s="258" t="s">
-        <v>209</v>
+        <v>231</v>
       </c>
       <c r="J25" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="M25" s="256" t="s">
         <v>389</v>
@@ -18178,11 +18193,11 @@
       </c>
     </row>
     <row r="26" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I26" s="258" t="s">
-        <v>232</v>
+      <c r="I26" s="257" t="s">
+        <v>936</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="M26" s="256" t="s">
         <v>390</v>
@@ -18196,10 +18211,10 @@
     </row>
     <row r="27" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I27" s="258" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J27" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M27" s="256" t="s">
         <v>391</v>
@@ -18212,11 +18227,11 @@
       </c>
     </row>
     <row r="28" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I28" s="257" t="s">
-        <v>937</v>
+      <c r="I28" s="258" t="s">
+        <v>232</v>
       </c>
       <c r="J28" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="M28" s="256" t="s">
         <v>392</v>
@@ -18230,10 +18245,10 @@
     </row>
     <row r="29" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I29" s="258" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J29" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M29" s="256" t="s">
         <v>393</v>
@@ -18247,10 +18262,10 @@
     </row>
     <row r="30" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I30" s="257" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="J30" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="M30" s="256" t="s">
         <v>874</v>
@@ -18264,10 +18279,10 @@
     </row>
     <row r="31" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I31" s="258" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J31" s="1" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="M31" s="256" t="s">
         <v>394</v>
@@ -18280,11 +18295,11 @@
       </c>
     </row>
     <row r="32" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I32" s="258" t="s">
-        <v>213</v>
-      </c>
-      <c r="J32" s="1" t="s">
-        <v>66</v>
+      <c r="I32" s="257" t="s">
+        <v>938</v>
+      </c>
+      <c r="J32" s="258" t="s">
+        <v>1060</v>
       </c>
       <c r="M32" s="256" t="s">
         <v>395</v>
@@ -18298,10 +18313,10 @@
     </row>
     <row r="33" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I33" s="258" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>76</v>
+        <v>89</v>
       </c>
       <c r="M33" s="256" t="s">
         <v>396</v>
@@ -18315,10 +18330,10 @@
     </row>
     <row r="34" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I34" s="258" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J34" s="1" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="M34" s="256" t="s">
         <v>397</v>
@@ -18332,10 +18347,10 @@
     </row>
     <row r="35" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I35" s="258" t="s">
-        <v>233</v>
+        <v>214</v>
       </c>
       <c r="J35" s="1" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="M35" s="256" t="s">
         <v>398</v>
@@ -18349,10 +18364,10 @@
     </row>
     <row r="36" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I36" s="258" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J36" s="1" t="s">
-        <v>85</v>
+        <v>54</v>
       </c>
       <c r="M36" s="256" t="s">
         <v>399</v>
@@ -18366,10 +18381,10 @@
     </row>
     <row r="37" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I37" s="258" t="s">
-        <v>217</v>
+        <v>233</v>
       </c>
       <c r="J37" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="M37" s="256" t="s">
         <v>875</v>
@@ -18383,10 +18398,10 @@
     </row>
     <row r="38" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I38" s="258" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J38" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="M38" s="256" t="s">
         <v>400</v>
@@ -18400,10 +18415,10 @@
     </row>
     <row r="39" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I39" s="258" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J39" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="M39" s="256" t="s">
         <v>401</v>
@@ -18417,7 +18432,10 @@
     </row>
     <row r="40" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I40" s="258" t="s">
-        <v>220</v>
+        <v>218</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="M40" s="256" t="s">
         <v>402</v>
@@ -18431,7 +18449,10 @@
     </row>
     <row r="41" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I41" s="258" t="s">
-        <v>221</v>
+        <v>219</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>88</v>
       </c>
       <c r="M41" s="256" t="s">
         <v>871</v>
@@ -18445,7 +18466,7 @@
     </row>
     <row r="42" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I42" s="258" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="M42" s="256" t="s">
         <v>404</v>
@@ -18459,7 +18480,7 @@
     </row>
     <row r="43" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I43" s="258" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="M43" s="256" t="s">
         <v>405</v>
@@ -18473,7 +18494,7 @@
     </row>
     <row r="44" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I44" s="258" t="s">
-        <v>228</v>
+        <v>1064</v>
       </c>
       <c r="M44" s="256" t="s">
         <v>406</v>
@@ -18487,7 +18508,7 @@
     </row>
     <row r="45" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I45" s="258" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="M45" s="256" t="s">
         <v>407</v>
@@ -18501,7 +18522,7 @@
     </row>
     <row r="46" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I46" s="258" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="M46" s="256" t="s">
         <v>408</v>
@@ -18515,7 +18536,7 @@
     </row>
     <row r="47" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I47" s="258" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="M47" s="256" t="s">
         <v>409</v>
@@ -18529,7 +18550,7 @@
     </row>
     <row r="48" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I48" s="258" t="s">
-        <v>225</v>
+        <v>229</v>
       </c>
       <c r="M48" s="256" t="s">
         <v>410</v>
@@ -18543,7 +18564,7 @@
     </row>
     <row r="49" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I49" s="258" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="M49" s="256" t="s">
         <v>411</v>
@@ -18557,7 +18578,7 @@
     </row>
     <row r="50" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I50" s="258" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="M50" s="256" t="s">
         <v>403</v>
@@ -18570,6 +18591,9 @@
       </c>
     </row>
     <row r="51" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I51" s="258" t="s">
+        <v>225</v>
+      </c>
       <c r="M51" s="256" t="s">
         <v>412</v>
       </c>
@@ -18581,6 +18605,9 @@
       </c>
     </row>
     <row r="52" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I52" s="258" t="s">
+        <v>226</v>
+      </c>
       <c r="M52" s="256" t="s">
         <v>413</v>
       </c>
@@ -18592,6 +18619,9 @@
       </c>
     </row>
     <row r="53" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="I53" s="258" t="s">
+        <v>227</v>
+      </c>
       <c r="M53" s="256" t="s">
         <v>414</v>
       </c>
@@ -18701,7 +18731,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="63" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+    <row r="63" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M63" s="256" t="s">
         <v>878</v>
       </c>
@@ -18723,7 +18753,7 @@
         <v>654</v>
       </c>
     </row>
-    <row r="65" spans="13:20" s="1" customFormat="1" ht="15.75" thickBot="1">
+    <row r="65" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="M65" s="256" t="s">
         <v>879</v>
       </c>
@@ -18734,7 +18764,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="66" spans="13:20" s="1" customFormat="1" ht="27" thickBot="1">
+    <row r="66" spans="9:20" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="M66" s="256" t="s">
         <v>423</v>
       </c>
@@ -18745,7 +18775,9 @@
         <v>911</v>
       </c>
     </row>
-    <row r="67" spans="13:20" ht="15.75" thickBot="1">
+    <row r="67" spans="9:20" ht="15.75" thickBot="1">
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
       <c r="M67" s="256" t="s">
         <v>424</v>
       </c>
@@ -18761,7 +18793,9 @@
       <c r="S67" s="1"/>
       <c r="T67" s="1"/>
     </row>
-    <row r="68" spans="13:20" ht="15.75" thickBot="1">
+    <row r="68" spans="9:20" ht="15.75" thickBot="1">
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
       <c r="M68" s="256" t="s">
         <v>425</v>
       </c>
@@ -18772,7 +18806,8 @@
         <v>623</v>
       </c>
     </row>
-    <row r="69" spans="13:20" ht="27" thickBot="1">
+    <row r="69" spans="9:20" ht="27" thickBot="1">
+      <c r="I69" s="1"/>
       <c r="M69" s="256" t="s">
         <v>881</v>
       </c>
@@ -18783,7 +18818,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="70" spans="13:20" ht="15.75" thickBot="1">
+    <row r="70" spans="9:20" ht="15.75" thickBot="1">
       <c r="M70" s="256" t="s">
         <v>882</v>
       </c>
@@ -18794,7 +18829,7 @@
         <v>625</v>
       </c>
     </row>
-    <row r="71" spans="13:20" ht="15.75" thickBot="1">
+    <row r="71" spans="9:20" ht="15.75" thickBot="1">
       <c r="M71" s="256" t="s">
         <v>426</v>
       </c>
@@ -18805,7 +18840,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="72" spans="13:20" ht="15.75" thickBot="1">
+    <row r="72" spans="9:20" ht="15.75" thickBot="1">
       <c r="M72" s="256" t="s">
         <v>427</v>
       </c>
@@ -18816,7 +18851,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="73" spans="13:20" ht="27" thickBot="1">
+    <row r="73" spans="9:20" ht="27" thickBot="1">
       <c r="M73" s="256" t="s">
         <v>428</v>
       </c>
@@ -18827,7 +18862,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="74" spans="13:20" ht="15.75" thickBot="1">
+    <row r="74" spans="9:20" ht="15.75" thickBot="1">
       <c r="M74" s="256" t="s">
         <v>429</v>
       </c>
@@ -18838,7 +18873,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="75" spans="13:20" ht="15.75" thickBot="1">
+    <row r="75" spans="9:20" ht="15.75" thickBot="1">
       <c r="M75" s="256" t="s">
         <v>883</v>
       </c>
@@ -18849,7 +18884,7 @@
         <v>915</v>
       </c>
     </row>
-    <row r="76" spans="13:20" ht="15.75" thickBot="1">
+    <row r="76" spans="9:20" ht="15.75" thickBot="1">
       <c r="M76" s="256" t="s">
         <v>431</v>
       </c>
@@ -18860,7 +18895,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="77" spans="13:20" ht="15.75" thickBot="1">
+    <row r="77" spans="9:20" ht="15.75" thickBot="1">
       <c r="M77" s="256" t="s">
         <v>430</v>
       </c>
@@ -18871,7 +18906,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="78" spans="13:20" ht="15.75" thickBot="1">
+    <row r="78" spans="9:20" ht="15.75" thickBot="1">
       <c r="M78" s="256" t="s">
         <v>432</v>
       </c>
@@ -18882,7 +18917,7 @@
         <v>917</v>
       </c>
     </row>
-    <row r="79" spans="13:20" ht="27" thickBot="1">
+    <row r="79" spans="9:20" ht="27" thickBot="1">
       <c r="M79" s="256" t="s">
         <v>433</v>
       </c>
@@ -18893,7 +18928,7 @@
         <v>630</v>
       </c>
     </row>
-    <row r="80" spans="13:20" ht="15.75" thickBot="1">
+    <row r="80" spans="9:20" ht="15.75" thickBot="1">
       <c r="M80" s="256" t="s">
         <v>434</v>
       </c>

</xml_diff>

<commit_message>
add 8 new crops: Castor bean, Chick pea, Coriander, Ginger, Pearl millet, Pomegranate, Sesame seed, Turmeric
</commit_message>
<xml_diff>
--- a/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
+++ b/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="DieseArbeitsmappe" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="1005" windowWidth="24240" windowHeight="13680" tabRatio="463"/>
+    <workbookView xWindow="120" yWindow="1005" windowWidth="24240" windowHeight="13680" tabRatio="463" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="127" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2341" uniqueCount="1080">
   <si>
     <t>Country</t>
   </si>
@@ -3538,6 +3538,30 @@
   </si>
   <si>
     <t>Strawberry processing grade</t>
+  </si>
+  <si>
+    <t>Castor bean</t>
+  </si>
+  <si>
+    <t>Chick pea</t>
+  </si>
+  <si>
+    <t>Coriander</t>
+  </si>
+  <si>
+    <t>Ginger</t>
+  </si>
+  <si>
+    <t>Pearl millet</t>
+  </si>
+  <si>
+    <t>Pomegranate</t>
+  </si>
+  <si>
+    <t>Sesame seed</t>
+  </si>
+  <si>
+    <t>Turmeric</t>
   </si>
 </sst>
 </file>
@@ -6168,6 +6192,18 @@
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="48" fillId="49" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="51" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="50" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -6182,18 +6218,6 @@
     </xf>
     <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="49" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="51" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="75" fillId="13" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="78" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -8345,7 +8369,7 @@
   </sheetPr>
   <dimension ref="A1:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView topLeftCell="A16" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="12.75"/>
   <cols>
@@ -8407,25 +8431,25 @@
     </row>
     <row r="5" spans="1:9" s="160" customFormat="1" ht="54.75" customHeight="1">
       <c r="A5" s="159"/>
-      <c r="B5" s="261"/>
-      <c r="C5" s="261"/>
-      <c r="D5" s="261"/>
-      <c r="E5" s="261"/>
-      <c r="F5" s="261"/>
-      <c r="G5" s="261"/>
+      <c r="B5" s="265"/>
+      <c r="C5" s="265"/>
+      <c r="D5" s="265"/>
+      <c r="E5" s="265"/>
+      <c r="F5" s="265"/>
+      <c r="G5" s="265"/>
       <c r="H5" s="156"/>
       <c r="I5" s="156"/>
     </row>
     <row r="6" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A6" s="154"/>
-      <c r="B6" s="262" t="s">
+      <c r="B6" s="266" t="s">
         <v>1036</v>
       </c>
-      <c r="C6" s="263"/>
-      <c r="D6" s="263"/>
-      <c r="E6" s="263"/>
-      <c r="F6" s="263"/>
-      <c r="G6" s="263"/>
+      <c r="C6" s="267"/>
+      <c r="D6" s="267"/>
+      <c r="E6" s="267"/>
+      <c r="F6" s="267"/>
+      <c r="G6" s="267"/>
       <c r="H6" s="156"/>
       <c r="I6" s="156"/>
     </row>
@@ -8442,14 +8466,14 @@
     </row>
     <row r="8" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A8" s="154"/>
-      <c r="B8" s="264" t="s">
+      <c r="B8" s="268" t="s">
         <v>702</v>
       </c>
-      <c r="C8" s="264"/>
-      <c r="D8" s="264"/>
-      <c r="E8" s="264"/>
-      <c r="F8" s="264"/>
-      <c r="G8" s="264"/>
+      <c r="C8" s="268"/>
+      <c r="D8" s="268"/>
+      <c r="E8" s="268"/>
+      <c r="F8" s="268"/>
+      <c r="G8" s="268"/>
       <c r="H8" s="161"/>
       <c r="I8" s="156"/>
     </row>
@@ -8466,14 +8490,14 @@
     </row>
     <row r="10" spans="1:9" s="157" customFormat="1" ht="12.95" customHeight="1">
       <c r="A10" s="154"/>
-      <c r="B10" s="265" t="s">
+      <c r="B10" s="269" t="s">
         <v>766</v>
       </c>
-      <c r="C10" s="265"/>
-      <c r="D10" s="265"/>
-      <c r="E10" s="265"/>
-      <c r="F10" s="265"/>
-      <c r="G10" s="265"/>
+      <c r="C10" s="269"/>
+      <c r="D10" s="269"/>
+      <c r="E10" s="269"/>
+      <c r="F10" s="269"/>
+      <c r="G10" s="269"/>
       <c r="H10" s="156"/>
       <c r="I10" s="156"/>
     </row>
@@ -8481,10 +8505,10 @@
       <c r="A11" s="154"/>
       <c r="B11" s="173"/>
       <c r="C11" s="173"/>
-      <c r="D11" s="265"/>
-      <c r="E11" s="265"/>
-      <c r="F11" s="265"/>
-      <c r="G11" s="265"/>
+      <c r="D11" s="269"/>
+      <c r="E11" s="269"/>
+      <c r="F11" s="269"/>
+      <c r="G11" s="269"/>
       <c r="H11" s="156"/>
       <c r="I11" s="156"/>
     </row>
@@ -8557,23 +8581,23 @@
     </row>
     <row r="17" spans="1:9" s="157" customFormat="1" ht="15.75">
       <c r="A17" s="154"/>
-      <c r="B17" s="267" t="s">
+      <c r="B17" s="262" t="s">
         <v>705</v>
       </c>
-      <c r="C17" s="267"/>
-      <c r="D17" s="267"/>
-      <c r="E17" s="267"/>
-      <c r="F17" s="267"/>
-      <c r="G17" s="267"/>
+      <c r="C17" s="262"/>
+      <c r="D17" s="262"/>
+      <c r="E17" s="262"/>
+      <c r="F17" s="262"/>
+      <c r="G17" s="262"/>
       <c r="H17" s="161"/>
       <c r="I17" s="156"/>
     </row>
     <row r="18" spans="1:9" s="160" customFormat="1">
       <c r="A18" s="159"/>
-      <c r="B18" s="268" t="s">
+      <c r="B18" s="263" t="s">
         <v>706</v>
       </c>
-      <c r="C18" s="268"/>
+      <c r="C18" s="263"/>
       <c r="D18" s="180" t="s">
         <v>707</v>
       </c>
@@ -8591,10 +8615,10 @@
     </row>
     <row r="19" spans="1:9" s="160" customFormat="1">
       <c r="A19" s="159"/>
-      <c r="B19" s="269" t="s">
+      <c r="B19" s="264" t="s">
         <v>711</v>
       </c>
-      <c r="C19" s="269"/>
+      <c r="C19" s="264"/>
       <c r="D19" s="166" t="s">
         <v>712</v>
       </c>
@@ -8633,10 +8657,10 @@
     </row>
     <row r="21" spans="1:9" s="160" customFormat="1">
       <c r="A21" s="159"/>
-      <c r="B21" s="266" t="s">
+      <c r="B21" s="261" t="s">
         <v>714</v>
       </c>
-      <c r="C21" s="266"/>
+      <c r="C21" s="261"/>
       <c r="D21" s="167" t="s">
         <v>715</v>
       </c>
@@ -8654,10 +8678,10 @@
     </row>
     <row r="22" spans="1:9" s="160" customFormat="1" ht="25.5">
       <c r="A22" s="159"/>
-      <c r="B22" s="266" t="s">
+      <c r="B22" s="261" t="s">
         <v>718</v>
       </c>
-      <c r="C22" s="266"/>
+      <c r="C22" s="261"/>
       <c r="D22" s="167" t="s">
         <v>719</v>
       </c>
@@ -8771,6 +8795,12 @@
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="D12:G12"/>
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B6:G6"/>
+    <mergeCell ref="B8:G8"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="D11:G11"/>
     <mergeCell ref="D13:G13"/>
     <mergeCell ref="D14:G14"/>
     <mergeCell ref="B21:C21"/>
@@ -8779,12 +8809,6 @@
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
     <mergeCell ref="D15:G15"/>
-    <mergeCell ref="D12:G12"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
-    <mergeCell ref="B8:G8"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="D11:G11"/>
   </mergeCells>
   <phoneticPr fontId="83" type="noConversion"/>
   <hyperlinks>
@@ -8807,9 +8831,9 @@
   <dimension ref="A1:Z245"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4:E4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="2"/>
@@ -12857,10 +12881,10 @@
   </sheetPr>
   <dimension ref="A1:AB225"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D4" sqref="D4"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -17274,7 +17298,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$I$2:$I$60</xm:f>
+            <xm:f>Lists!$I$2:$I$68</xm:f>
           </x14:formula1>
           <xm:sqref>D4</xm:sqref>
         </x14:dataValidation>
@@ -17292,9 +17316,9 @@
   <dimension ref="A1:V141"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B35" sqref="B35"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="I2" sqref="I2:I68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -17396,7 +17420,7 @@
       <c r="H2" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="258" t="s">
         <v>654</v>
       </c>
       <c r="J2" s="1" t="s">
@@ -17996,7 +18020,7 @@
     </row>
     <row r="16" spans="1:22" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I16" s="257" t="s">
-        <v>922</v>
+        <v>1072</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>64</v>
@@ -18019,8 +18043,8 @@
       </c>
     </row>
     <row r="17" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I17" s="258" t="s">
-        <v>199</v>
+      <c r="I17" s="257" t="s">
+        <v>1073</v>
       </c>
       <c r="J17" s="1" t="s">
         <v>69</v>
@@ -18043,8 +18067,8 @@
       </c>
     </row>
     <row r="18" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I18" s="258" t="s">
-        <v>202</v>
+      <c r="I18" s="257" t="s">
+        <v>922</v>
       </c>
       <c r="J18" s="1" t="s">
         <v>70</v>
@@ -18068,7 +18092,7 @@
     </row>
     <row r="19" spans="9:20" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I19" s="258" t="s">
-        <v>1069</v>
+        <v>199</v>
       </c>
       <c r="J19" s="1" t="s">
         <v>73</v>
@@ -18092,7 +18116,7 @@
     </row>
     <row r="20" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I20" s="258" t="s">
-        <v>1068</v>
+        <v>202</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>71</v>
@@ -18115,8 +18139,8 @@
       </c>
     </row>
     <row r="21" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I21" s="257" t="s">
-        <v>923</v>
+      <c r="I21" s="258" t="s">
+        <v>1069</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>72</v>
@@ -18139,8 +18163,8 @@
       </c>
     </row>
     <row r="22" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I22" s="257" t="s">
-        <v>1056</v>
+      <c r="I22" s="258" t="s">
+        <v>1074</v>
       </c>
       <c r="J22" s="1" t="s">
         <v>74</v>
@@ -18163,8 +18187,8 @@
       </c>
     </row>
     <row r="23" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I23" s="257" t="s">
-        <v>924</v>
+      <c r="I23" s="258" t="s">
+        <v>1068</v>
       </c>
       <c r="J23" s="1" t="s">
         <v>75</v>
@@ -18181,7 +18205,7 @@
     </row>
     <row r="24" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I24" s="257" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="J24" s="258" t="s">
         <v>1054</v>
@@ -18198,7 +18222,7 @@
     </row>
     <row r="25" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I25" s="257" t="s">
-        <v>926</v>
+        <v>1056</v>
       </c>
       <c r="J25" s="1" t="s">
         <v>77</v>
@@ -18215,7 +18239,7 @@
     </row>
     <row r="26" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I26" s="257" t="s">
-        <v>927</v>
+        <v>924</v>
       </c>
       <c r="J26" s="1" t="s">
         <v>78</v>
@@ -18232,7 +18256,7 @@
     </row>
     <row r="27" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I27" s="257" t="s">
-        <v>928</v>
+        <v>925</v>
       </c>
       <c r="J27" s="1" t="s">
         <v>79</v>
@@ -18249,7 +18273,7 @@
     </row>
     <row r="28" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I28" s="257" t="s">
-        <v>1062</v>
+        <v>1075</v>
       </c>
       <c r="J28" s="1" t="s">
         <v>80</v>
@@ -18265,8 +18289,8 @@
       </c>
     </row>
     <row r="29" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I29" s="258" t="s">
-        <v>1063</v>
+      <c r="I29" s="257" t="s">
+        <v>926</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>81</v>
@@ -18283,7 +18307,7 @@
     </row>
     <row r="30" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I30" s="257" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="J30" s="1" t="s">
         <v>82</v>
@@ -18299,8 +18323,8 @@
       </c>
     </row>
     <row r="31" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I31" s="258" t="s">
-        <v>207</v>
+      <c r="I31" s="257" t="s">
+        <v>928</v>
       </c>
       <c r="J31" s="1" t="s">
         <v>83</v>
@@ -18316,8 +18340,8 @@
       </c>
     </row>
     <row r="32" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I32" s="258" t="s">
-        <v>226</v>
+      <c r="I32" s="257" t="s">
+        <v>1062</v>
       </c>
       <c r="J32" s="258" t="s">
         <v>1053</v>
@@ -18334,7 +18358,7 @@
     </row>
     <row r="33" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I33" s="258" t="s">
-        <v>208</v>
+        <v>1063</v>
       </c>
       <c r="J33" s="1" t="s">
         <v>89</v>
@@ -18351,7 +18375,7 @@
     </row>
     <row r="34" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I34" s="257" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="J34" s="1" t="s">
         <v>66</v>
@@ -18368,7 +18392,7 @@
     </row>
     <row r="35" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I35" s="258" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J35" s="1" t="s">
         <v>76</v>
@@ -18384,8 +18408,8 @@
       </c>
     </row>
     <row r="36" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
-      <c r="I36" s="257" t="s">
-        <v>931</v>
+      <c r="I36" s="258" t="s">
+        <v>226</v>
       </c>
       <c r="J36" s="1" t="s">
         <v>54</v>
@@ -18402,7 +18426,7 @@
     </row>
     <row r="37" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I37" s="258" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J37" s="1" t="s">
         <v>84</v>
@@ -18418,8 +18442,8 @@
       </c>
     </row>
     <row r="38" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I38" s="258" t="s">
-        <v>211</v>
+      <c r="I38" s="257" t="s">
+        <v>930</v>
       </c>
       <c r="J38" s="1" t="s">
         <v>85</v>
@@ -18436,7 +18460,7 @@
     </row>
     <row r="39" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I39" s="258" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="J39" s="1" t="s">
         <v>86</v>
@@ -18452,8 +18476,8 @@
       </c>
     </row>
     <row r="40" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
-      <c r="I40" s="258" t="s">
-        <v>1064</v>
+      <c r="I40" s="257" t="s">
+        <v>931</v>
       </c>
       <c r="J40" s="1" t="s">
         <v>87</v>
@@ -18470,7 +18494,7 @@
     </row>
     <row r="41" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I41" s="258" t="s">
-        <v>1065</v>
+        <v>210</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>88</v>
@@ -18487,7 +18511,7 @@
     </row>
     <row r="42" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I42" s="258" t="s">
-        <v>227</v>
+        <v>211</v>
       </c>
       <c r="M42" s="256" t="s">
         <v>398</v>
@@ -18501,7 +18525,7 @@
     </row>
     <row r="43" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I43" s="258" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="M43" s="256" t="s">
         <v>399</v>
@@ -18515,7 +18539,7 @@
     </row>
     <row r="44" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I44" s="258" t="s">
-        <v>214</v>
+        <v>1064</v>
       </c>
       <c r="M44" s="256" t="s">
         <v>400</v>
@@ -18529,7 +18553,7 @@
     </row>
     <row r="45" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I45" s="258" t="s">
-        <v>215</v>
+        <v>1065</v>
       </c>
       <c r="M45" s="256" t="s">
         <v>401</v>
@@ -18543,7 +18567,7 @@
     </row>
     <row r="46" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I46" s="258" t="s">
-        <v>216</v>
+        <v>227</v>
       </c>
       <c r="M46" s="256" t="s">
         <v>402</v>
@@ -18557,7 +18581,7 @@
     </row>
     <row r="47" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I47" s="258" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="M47" s="256" t="s">
         <v>403</v>
@@ -18571,7 +18595,7 @@
     </row>
     <row r="48" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I48" s="258" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="M48" s="256" t="s">
         <v>404</v>
@@ -18585,7 +18609,7 @@
     </row>
     <row r="49" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I49" s="258" t="s">
-        <v>1057</v>
+        <v>215</v>
       </c>
       <c r="M49" s="256" t="s">
         <v>405</v>
@@ -18599,7 +18623,7 @@
     </row>
     <row r="50" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I50" s="258" t="s">
-        <v>219</v>
+        <v>1076</v>
       </c>
       <c r="M50" s="256" t="s">
         <v>397</v>
@@ -18613,7 +18637,7 @@
     </row>
     <row r="51" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I51" s="258" t="s">
-        <v>1070</v>
+        <v>216</v>
       </c>
       <c r="M51" s="256" t="s">
         <v>406</v>
@@ -18627,7 +18651,7 @@
     </row>
     <row r="52" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I52" s="258" t="s">
-        <v>1071</v>
+        <v>1077</v>
       </c>
       <c r="M52" s="256" t="s">
         <v>407</v>
@@ -18641,7 +18665,7 @@
     </row>
     <row r="53" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I53" s="258" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="M53" s="256" t="s">
         <v>408</v>
@@ -18655,7 +18679,7 @@
     </row>
     <row r="54" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I54" s="258" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="M54" s="256" t="s">
         <v>409</v>
@@ -18669,7 +18693,7 @@
     </row>
     <row r="55" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I55" s="258" t="s">
-        <v>220</v>
+        <v>1057</v>
       </c>
       <c r="M55" s="256" t="s">
         <v>870</v>
@@ -18683,7 +18707,7 @@
     </row>
     <row r="56" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
       <c r="I56" s="258" t="s">
-        <v>225</v>
+        <v>1078</v>
       </c>
       <c r="M56" s="256" t="s">
         <v>871</v>
@@ -18697,7 +18721,7 @@
     </row>
     <row r="57" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I57" s="258" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="M57" s="256" t="s">
         <v>410</v>
@@ -18711,7 +18735,7 @@
     </row>
     <row r="58" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I58" s="258" t="s">
-        <v>1066</v>
+        <v>1070</v>
       </c>
       <c r="M58" s="256" t="s">
         <v>411</v>
@@ -18725,7 +18749,7 @@
     </row>
     <row r="59" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I59" s="258" t="s">
-        <v>1067</v>
+        <v>1071</v>
       </c>
       <c r="M59" s="256" t="s">
         <v>412</v>
@@ -18739,7 +18763,7 @@
     </row>
     <row r="60" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
       <c r="I60" s="258" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="M60" s="256" t="s">
         <v>413</v>
@@ -18752,6 +18776,9 @@
       </c>
     </row>
     <row r="61" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I61" s="258" t="s">
+        <v>224</v>
+      </c>
       <c r="M61" s="256" t="s">
         <v>414</v>
       </c>
@@ -18763,6 +18790,9 @@
       </c>
     </row>
     <row r="62" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I62" s="258" t="s">
+        <v>220</v>
+      </c>
       <c r="M62" s="256" t="s">
         <v>415</v>
       </c>
@@ -18774,6 +18804,9 @@
       </c>
     </row>
     <row r="63" spans="9:15" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="I63" s="258" t="s">
+        <v>225</v>
+      </c>
       <c r="M63" s="256" t="s">
         <v>872</v>
       </c>
@@ -18785,6 +18818,9 @@
       </c>
     </row>
     <row r="64" spans="9:15" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I64" s="258" t="s">
+        <v>221</v>
+      </c>
       <c r="M64" s="256" t="s">
         <v>416</v>
       </c>
@@ -18796,6 +18832,9 @@
       </c>
     </row>
     <row r="65" spans="9:20" s="1" customFormat="1" ht="15.75" thickBot="1">
+      <c r="I65" s="258" t="s">
+        <v>1066</v>
+      </c>
       <c r="M65" s="256" t="s">
         <v>873</v>
       </c>
@@ -18807,6 +18846,9 @@
       </c>
     </row>
     <row r="66" spans="9:20" s="1" customFormat="1" ht="27" thickBot="1">
+      <c r="I66" s="258" t="s">
+        <v>1067</v>
+      </c>
       <c r="M66" s="256" t="s">
         <v>417</v>
       </c>
@@ -18818,7 +18860,9 @@
       </c>
     </row>
     <row r="67" spans="9:20" ht="15.75" thickBot="1">
-      <c r="I67" s="1"/>
+      <c r="I67" s="258" t="s">
+        <v>1079</v>
+      </c>
       <c r="J67" s="1"/>
       <c r="M67" s="256" t="s">
         <v>418</v>
@@ -18836,7 +18880,9 @@
       <c r="T67" s="1"/>
     </row>
     <row r="68" spans="9:20" ht="15.75" thickBot="1">
-      <c r="I68" s="1"/>
+      <c r="I68" s="258" t="s">
+        <v>222</v>
+      </c>
       <c r="J68" s="1"/>
       <c r="M68" s="256" t="s">
         <v>419</v>

</xml_diff>

<commit_message>
ecoinvent template: put zero when we don't want default values
</commit_message>
<xml_diff>
--- a/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
+++ b/src/main/dart/web/LCI-Database_Data-collection_Crop_v2.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2155" uniqueCount="971">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2149" uniqueCount="971">
   <si>
     <t>Country</t>
   </si>
@@ -5440,26 +5440,26 @@
     <xf numFmtId="0" fontId="72" fillId="9" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="77" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="47" fillId="24" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="72" fillId="9" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="72" fillId="9" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="47" fillId="24" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="79" fillId="23" borderId="0" xfId="27" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="77" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="6" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="72" fillId="9" borderId="0" xfId="27" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="80" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1" indent="2"/>
@@ -7585,27 +7585,27 @@
     </row>
     <row r="2" spans="1:9" s="112" customFormat="1" ht="51.75" customHeight="1">
       <c r="A2" s="111"/>
-      <c r="B2" s="213" t="s">
+      <c r="B2" s="210" t="s">
         <v>943</v>
       </c>
-      <c r="C2" s="213"/>
-      <c r="D2" s="213"/>
-      <c r="E2" s="213"/>
-      <c r="F2" s="213"/>
-      <c r="G2" s="213"/>
+      <c r="C2" s="210"/>
+      <c r="D2" s="210"/>
+      <c r="E2" s="210"/>
+      <c r="F2" s="210"/>
+      <c r="G2" s="210"/>
       <c r="H2" s="109"/>
       <c r="I2" s="109"/>
     </row>
     <row r="3" spans="1:9" s="110" customFormat="1" ht="12.95" customHeight="1">
       <c r="A3" s="107"/>
-      <c r="B3" s="214" t="s">
+      <c r="B3" s="211" t="s">
         <v>903</v>
       </c>
-      <c r="C3" s="215"/>
-      <c r="D3" s="215"/>
-      <c r="E3" s="215"/>
-      <c r="F3" s="215"/>
-      <c r="G3" s="215"/>
+      <c r="C3" s="212"/>
+      <c r="D3" s="212"/>
+      <c r="E3" s="212"/>
+      <c r="F3" s="212"/>
+      <c r="G3" s="212"/>
       <c r="H3" s="109"/>
       <c r="I3" s="109"/>
     </row>
@@ -7622,14 +7622,14 @@
     </row>
     <row r="5" spans="1:9" s="110" customFormat="1" ht="15.75">
       <c r="A5" s="107"/>
-      <c r="B5" s="211" t="s">
+      <c r="B5" s="213" t="s">
         <v>620</v>
       </c>
-      <c r="C5" s="211"/>
-      <c r="D5" s="211"/>
-      <c r="E5" s="211"/>
-      <c r="F5" s="211"/>
-      <c r="G5" s="211"/>
+      <c r="C5" s="213"/>
+      <c r="D5" s="213"/>
+      <c r="E5" s="213"/>
+      <c r="F5" s="213"/>
+      <c r="G5" s="213"/>
       <c r="H5" s="113"/>
       <c r="I5" s="109"/>
     </row>
@@ -7646,14 +7646,14 @@
     </row>
     <row r="7" spans="1:9" s="110" customFormat="1" ht="12.95" customHeight="1">
       <c r="A7" s="107"/>
-      <c r="B7" s="216" t="s">
+      <c r="B7" s="214" t="s">
         <v>669</v>
       </c>
-      <c r="C7" s="216"/>
-      <c r="D7" s="216"/>
-      <c r="E7" s="216"/>
-      <c r="F7" s="216"/>
-      <c r="G7" s="216"/>
+      <c r="C7" s="214"/>
+      <c r="D7" s="214"/>
+      <c r="E7" s="214"/>
+      <c r="F7" s="214"/>
+      <c r="G7" s="214"/>
       <c r="H7" s="109"/>
       <c r="I7" s="109"/>
     </row>
@@ -7661,10 +7661,10 @@
       <c r="A8" s="107"/>
       <c r="B8" s="125"/>
       <c r="C8" s="125"/>
-      <c r="D8" s="216"/>
-      <c r="E8" s="216"/>
-      <c r="F8" s="216"/>
-      <c r="G8" s="216"/>
+      <c r="D8" s="214"/>
+      <c r="E8" s="214"/>
+      <c r="F8" s="214"/>
+      <c r="G8" s="214"/>
       <c r="H8" s="109"/>
       <c r="I8" s="109"/>
     </row>
@@ -7737,23 +7737,23 @@
     </row>
     <row r="14" spans="1:9" s="110" customFormat="1" ht="15.75">
       <c r="A14" s="107"/>
-      <c r="B14" s="211" t="s">
+      <c r="B14" s="213" t="s">
         <v>623</v>
       </c>
-      <c r="C14" s="211"/>
-      <c r="D14" s="211"/>
-      <c r="E14" s="211"/>
-      <c r="F14" s="211"/>
-      <c r="G14" s="211"/>
+      <c r="C14" s="213"/>
+      <c r="D14" s="213"/>
+      <c r="E14" s="213"/>
+      <c r="F14" s="213"/>
+      <c r="G14" s="213"/>
       <c r="H14" s="113"/>
       <c r="I14" s="109"/>
     </row>
     <row r="15" spans="1:9" s="112" customFormat="1">
       <c r="A15" s="111"/>
-      <c r="B15" s="212" t="s">
+      <c r="B15" s="216" t="s">
         <v>624</v>
       </c>
-      <c r="C15" s="212"/>
+      <c r="C15" s="216"/>
       <c r="D15" s="191" t="s">
         <v>625</v>
       </c>
@@ -7792,10 +7792,10 @@
     </row>
     <row r="17" spans="1:9" s="112" customFormat="1" ht="25.5">
       <c r="A17" s="111"/>
-      <c r="B17" s="210" t="s">
+      <c r="B17" s="215" t="s">
         <v>629</v>
       </c>
-      <c r="C17" s="210"/>
+      <c r="C17" s="215"/>
       <c r="D17" s="119" t="s">
         <v>630</v>
       </c>
@@ -7909,18 +7909,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="D10:G10"/>
+    <mergeCell ref="D11:G11"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="D12:G12"/>
     <mergeCell ref="D9:G9"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B5:G5"/>
     <mergeCell ref="B7:G7"/>
     <mergeCell ref="D8:G8"/>
-    <mergeCell ref="D10:G10"/>
-    <mergeCell ref="D11:G11"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="D12:G12"/>
   </mergeCells>
   <phoneticPr fontId="76" type="noConversion"/>
   <hyperlinks>
@@ -7981,7 +7981,7 @@
       <c r="F2" s="44"/>
     </row>
     <row r="3" spans="1:8" s="11" customFormat="1" ht="61.5" customHeight="1">
-      <c r="B3" s="213" t="s">
+      <c r="B3" s="210" t="s">
         <v>943</v>
       </c>
       <c r="C3" s="217"/>
@@ -11445,7 +11445,7 @@
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="7" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="C16" sqref="C16"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <selection pane="bottomLeft" sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.85546875" defaultRowHeight="15" outlineLevelRow="1"/>
@@ -11491,14 +11491,14 @@
       <c r="G2" s="221"/>
     </row>
     <row r="3" spans="1:8" s="11" customFormat="1" ht="61.5" customHeight="1">
-      <c r="B3" s="213" t="s">
+      <c r="B3" s="210" t="s">
         <v>943</v>
       </c>
-      <c r="C3" s="213"/>
-      <c r="D3" s="213"/>
-      <c r="E3" s="213"/>
-      <c r="F3" s="213"/>
-      <c r="G3" s="213"/>
+      <c r="C3" s="210"/>
+      <c r="D3" s="210"/>
+      <c r="E3" s="210"/>
+      <c r="F3" s="210"/>
+      <c r="G3" s="210"/>
     </row>
     <row r="4" spans="1:8" s="11" customFormat="1" ht="15.95" customHeight="1">
       <c r="B4" s="176"/>
@@ -12174,8 +12174,8 @@
       <c r="D45" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E45" s="80" t="s">
-        <v>91</v>
+      <c r="E45" s="80">
+        <v>0</v>
       </c>
       <c r="F45" s="3"/>
       <c r="G45" s="37"/>
@@ -12380,8 +12380,8 @@
       <c r="D57" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="E57" s="80" t="s">
-        <v>91</v>
+      <c r="E57" s="80">
+        <v>0</v>
       </c>
       <c r="F57" s="3"/>
       <c r="G57" s="39"/>
@@ -12535,8 +12535,8 @@
       <c r="D66" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E66" s="80" t="s">
-        <v>91</v>
+      <c r="E66" s="80">
+        <v>0</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="37"/>
@@ -12951,8 +12951,8 @@
       <c r="D90" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E90" s="80" t="s">
-        <v>91</v>
+      <c r="E90" s="80">
+        <v>0</v>
       </c>
       <c r="F90" s="3"/>
       <c r="G90" s="31"/>
@@ -13036,8 +13036,8 @@
       <c r="D95" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E95" s="80" t="s">
-        <v>91</v>
+      <c r="E95" s="80">
+        <v>0</v>
       </c>
       <c r="F95" s="3"/>
       <c r="G95" s="31"/>
@@ -13270,8 +13270,8 @@
       <c r="D109" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="E109" s="82" t="s">
-        <v>91</v>
+      <c r="E109" s="82">
+        <v>0</v>
       </c>
       <c r="F109" s="40"/>
       <c r="G109" s="3"/>

</xml_diff>